<commit_message>
August 5 forecast update
</commit_message>
<xml_diff>
--- a/Forecast/TCs_within_50_miles_1880-2020.xlsx
+++ b/Forecast/TCs_within_50_miles_1880-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmbell/Development/csu-tropical/Forecast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B83AE59-A5B6-E049-A7DC-3618527EAE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CE2424-AA7A-DF48-8960-AC439E6E4DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="2740" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="County" sheetId="1" r:id="rId1"/>
@@ -1071,7 +1071,7 @@
         <v>231</v>
       </c>
       <c r="B1" s="14">
-        <v>170</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1169,15 +1169,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="19">
         <f>(1-(1/(2.71828^((C5*($B$1/100))/141))))</f>
-        <v>0.37513049913771845</v>
+        <v>0.32667802677005708</v>
       </c>
       <c r="H5" s="19">
         <f t="shared" ref="H5" si="0">(1-(1/(2.71828^((D5*($B$1/100))/141))))</f>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="I5" s="19">
         <f>IF(E5*($B$1/100)&gt;0, (1-(1/(2.71828^(E5*($B$1/100)/141)))), "&lt;1%")</f>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K5" s="2">
         <f>(1-(1/(2.71828^(C5/141))))</f>
@@ -1211,15 +1211,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="19">
         <f t="shared" ref="G6:G69" si="1">(1-(1/(2.71828^((C6*($B$1/100))/141))))</f>
-        <v>0.34425647321583208</v>
+        <v>0.2988015246204283</v>
       </c>
       <c r="H6" s="19">
         <f t="shared" ref="H6:H69" si="2">(1-(1/(2.71828^((D6*($B$1/100))/141))))</f>
-        <v>0.2047333884389867</v>
+        <v>0.17526644285268</v>
       </c>
       <c r="I6" s="19">
         <f t="shared" ref="I6:I69" si="3">IF(E6*($B$1/100)&gt;0, (1-(1/(2.71828^(E6*($B$1/100)/141)))), "&lt;1%")</f>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ref="K6:K69" si="4">(1-(1/(2.71828^(C6/141))))</f>
@@ -1253,15 +1253,15 @@
       <c r="F7" s="6"/>
       <c r="G7" s="19">
         <f t="shared" si="1"/>
-        <v>0.37513049913771845</v>
+        <v>0.32667802677005708</v>
       </c>
       <c r="H7" s="19">
         <f t="shared" si="2"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="I7" s="19">
         <f t="shared" si="3"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ref="K7" si="7">(1-(1/(2.71828^(C7/141))))</f>
@@ -1294,15 +1294,15 @@
       </c>
       <c r="G8" s="19">
         <f t="shared" si="1"/>
-        <v>0.3521151255059447</v>
+        <v>0.30587702543196937</v>
       </c>
       <c r="H8" s="19">
         <f t="shared" si="2"/>
-        <v>0.2047333884389867</v>
+        <v>0.17526644285268</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="4"/>
@@ -1335,15 +1335,15 @@
       </c>
       <c r="G9" s="19">
         <f t="shared" si="1"/>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="H9" s="19">
         <f t="shared" si="2"/>
-        <v>0.18532368255428877</v>
+        <v>0.15836700404317228</v>
       </c>
       <c r="I9" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="4"/>
@@ -1376,15 +1376,15 @@
       </c>
       <c r="G10" s="19">
         <f t="shared" si="1"/>
-        <v>0.37513049913771845</v>
+        <v>0.32667802677005708</v>
       </c>
       <c r="H10" s="19">
         <f t="shared" si="2"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="I10" s="19">
         <f t="shared" si="3"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="4"/>
@@ -1417,15 +1417,15 @@
       </c>
       <c r="G11" s="19">
         <f t="shared" si="1"/>
-        <v>0.30351002855087539</v>
+        <v>0.26232734853940509</v>
       </c>
       <c r="H11" s="19">
         <f t="shared" si="2"/>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="I11" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="4"/>
@@ -1458,15 +1458,15 @@
       </c>
       <c r="G12" s="19">
         <f t="shared" si="1"/>
-        <v>0.39001804768716197</v>
+        <v>0.34019789058285854</v>
       </c>
       <c r="H12" s="19">
         <f t="shared" si="2"/>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="I12" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" si="4"/>
@@ -1499,15 +1499,15 @@
       </c>
       <c r="G13" s="19">
         <f t="shared" si="1"/>
-        <v>0.47850906740128607</v>
+        <v>0.42169808713392831</v>
       </c>
       <c r="H13" s="19">
         <f t="shared" si="2"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="I13" s="19">
         <f t="shared" si="3"/>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="4"/>
@@ -1540,15 +1540,15 @@
       </c>
       <c r="G14" s="19">
         <f t="shared" si="1"/>
-        <v>0.45930136300416158</v>
+        <v>0.40383254978091254</v>
       </c>
       <c r="H14" s="19">
         <f t="shared" si="2"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="I14" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="4"/>
@@ -1581,15 +1581,15 @@
       </c>
       <c r="G15" s="19">
         <f t="shared" si="1"/>
-        <v>0.50306214938143157</v>
+        <v>0.44468877391261652</v>
       </c>
       <c r="H15" s="19">
         <f t="shared" si="2"/>
-        <v>0.29506181078156346</v>
+        <v>0.25480792671460639</v>
       </c>
       <c r="I15" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="4"/>
@@ -1622,15 +1622,15 @@
       </c>
       <c r="G16" s="19">
         <f t="shared" si="1"/>
-        <v>0.45930136300416158</v>
+        <v>0.40383254978091254</v>
       </c>
       <c r="H16" s="19">
         <f t="shared" si="2"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="I16" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="4"/>
@@ -1663,15 +1663,15 @@
       </c>
       <c r="G17" s="19">
         <f t="shared" si="1"/>
-        <v>0.4461047804194278</v>
+        <v>0.39161661015060845</v>
       </c>
       <c r="H17" s="19">
         <f t="shared" si="2"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="I17" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="4"/>
@@ -1704,15 +1704,15 @@
       </c>
       <c r="G18" s="19">
         <f t="shared" si="1"/>
-        <v>0.4461047804194278</v>
+        <v>0.39161661015060845</v>
       </c>
       <c r="H18" s="19">
         <f t="shared" si="2"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="I18" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="4"/>
@@ -1745,15 +1745,15 @@
       </c>
       <c r="G19" s="19">
         <f t="shared" si="1"/>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="H19" s="19">
         <f t="shared" si="2"/>
-        <v>0.15531728952486967</v>
+        <v>0.1323663538771066</v>
       </c>
       <c r="I19" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="4"/>
@@ -1786,15 +1786,15 @@
       </c>
       <c r="G20" s="19">
         <f t="shared" si="1"/>
-        <v>0.47218353631840626</v>
+        <v>0.41580320135184334</v>
       </c>
       <c r="H20" s="19">
         <f t="shared" si="2"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="I20" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="4"/>
@@ -1827,15 +1827,15 @@
       </c>
       <c r="G21" s="19">
         <f t="shared" si="1"/>
-        <v>0.46578127841061079</v>
+        <v>0.4098482264059311</v>
       </c>
       <c r="H21" s="19">
         <f t="shared" si="2"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="I21" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="4"/>
@@ -1868,15 +1868,15 @@
       </c>
       <c r="G22" s="19">
         <f t="shared" si="1"/>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="H22" s="19">
         <f t="shared" si="2"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="I22" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" si="4"/>
@@ -1909,15 +1909,15 @@
       </c>
       <c r="G23" s="19">
         <f t="shared" si="1"/>
-        <v>0.52071530159105595</v>
+        <v>0.46132995995618065</v>
       </c>
       <c r="H23" s="19">
         <f t="shared" si="2"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="I23" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K23" s="2">
         <f t="shared" si="4"/>
@@ -1950,15 +1950,15 @@
       </c>
       <c r="G24" s="19">
         <f t="shared" si="1"/>
-        <v>0.61421753432852066</v>
+        <v>0.55121221170521451</v>
       </c>
       <c r="H24" s="19">
         <f t="shared" si="2"/>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="I24" s="19">
         <f t="shared" si="3"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="4"/>
@@ -1991,15 +1991,15 @@
       </c>
       <c r="G25" s="19">
         <f t="shared" si="1"/>
-        <v>0.57515368744915019</v>
+        <v>0.51328202850696369</v>
       </c>
       <c r="H25" s="19">
         <f t="shared" si="2"/>
-        <v>0.32825204299627064</v>
+        <v>0.28443341673236711</v>
       </c>
       <c r="I25" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K25" s="2">
         <f t="shared" si="4"/>
@@ -2032,15 +2032,15 @@
       </c>
       <c r="G26" s="19">
         <f t="shared" si="1"/>
-        <v>0.5541625588240332</v>
+        <v>0.4931312015355781</v>
       </c>
       <c r="H26" s="19">
         <f t="shared" si="2"/>
-        <v>0.30351002855087539</v>
+        <v>0.26232734853940509</v>
       </c>
       <c r="I26" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="4"/>
@@ -2073,15 +2073,15 @@
       </c>
       <c r="G27" s="19">
         <f t="shared" si="1"/>
-        <v>0.61884088192327691</v>
+        <v>0.55574074174597166</v>
       </c>
       <c r="H27" s="19">
         <f t="shared" si="2"/>
-        <v>0.34425647321583208</v>
+        <v>0.2988015246204283</v>
       </c>
       <c r="I27" s="19">
         <f t="shared" si="3"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="4"/>
@@ -2114,15 +2114,15 @@
       </c>
       <c r="G28" s="19">
         <f t="shared" si="1"/>
-        <v>0.59024586972470483</v>
+        <v>0.52786765893159926</v>
       </c>
       <c r="H28" s="19">
         <f t="shared" si="2"/>
-        <v>0.32825204299627064</v>
+        <v>0.28443341673236711</v>
       </c>
       <c r="I28" s="19">
         <f t="shared" si="3"/>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" si="4"/>
@@ -2155,15 +2155,15 @@
       </c>
       <c r="G29" s="19">
         <f t="shared" si="1"/>
-        <v>0.47850906740128607</v>
+        <v>0.42169808713392831</v>
       </c>
       <c r="H29" s="19">
         <f t="shared" si="2"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="I29" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K29" s="2">
         <f t="shared" si="4"/>
@@ -2196,15 +2196,15 @@
       </c>
       <c r="G30" s="19">
         <f t="shared" si="1"/>
-        <v>0.50306214938143157</v>
+        <v>0.44468877391261652</v>
       </c>
       <c r="H30" s="19">
         <f t="shared" si="2"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="I30" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" si="4"/>
@@ -2237,15 +2237,15 @@
       </c>
       <c r="G31" s="19">
         <f t="shared" si="1"/>
-        <v>0.47850906740128607</v>
+        <v>0.42169808713392831</v>
       </c>
       <c r="H31" s="19">
         <f t="shared" si="2"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I31" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" si="4"/>
@@ -2278,15 +2278,15 @@
       </c>
       <c r="G32" s="19">
         <f t="shared" si="1"/>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="H32" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I32" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="4"/>
@@ -2319,15 +2319,15 @@
       </c>
       <c r="G33" s="19">
         <f t="shared" si="1"/>
-        <v>0.48475879117948029</v>
+        <v>0.42753349008682928</v>
       </c>
       <c r="H33" s="19">
         <f t="shared" si="2"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="I33" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="4"/>
@@ -2360,15 +2360,15 @@
       </c>
       <c r="G34" s="19">
         <f t="shared" si="1"/>
-        <v>0.5541625588240332</v>
+        <v>0.4931312015355781</v>
       </c>
       <c r="H34" s="19">
         <f t="shared" si="2"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="I34" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" si="4"/>
@@ -2401,15 +2401,15 @@
       </c>
       <c r="G35" s="19">
         <f t="shared" si="1"/>
-        <v>0.59515650185867774</v>
+        <v>0.53263174909961608</v>
       </c>
       <c r="H35" s="19">
         <f t="shared" si="2"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="I35" s="19">
         <f t="shared" si="3"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="4"/>
@@ -2442,15 +2442,15 @@
       </c>
       <c r="G36" s="19">
         <f t="shared" si="1"/>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="H36" s="19">
         <f t="shared" si="2"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="I36" s="19">
         <f t="shared" si="3"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" si="4"/>
@@ -2483,15 +2483,15 @@
       </c>
       <c r="G37" s="19">
         <f t="shared" si="1"/>
-        <v>0.52071530159105595</v>
+        <v>0.46132995995618065</v>
       </c>
       <c r="H37" s="19">
         <f t="shared" si="2"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="I37" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K37" s="2">
         <f t="shared" si="4"/>
@@ -2524,15 +2524,15 @@
       </c>
       <c r="G38" s="19">
         <f t="shared" si="1"/>
-        <v>0.52645921157860687</v>
+        <v>0.46676545424104743</v>
       </c>
       <c r="H38" s="19">
         <f t="shared" si="2"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="I38" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K38" s="2">
         <f t="shared" si="4"/>
@@ -2565,15 +2565,15 @@
       </c>
       <c r="G39" s="19">
         <f t="shared" si="1"/>
-        <v>0.51490171967079768</v>
+        <v>0.45583905928709567</v>
       </c>
       <c r="H39" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I39" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K39" s="2">
         <f t="shared" si="4"/>
@@ -2606,15 +2606,15 @@
       </c>
       <c r="G40" s="19">
         <f t="shared" si="1"/>
-        <v>0.50306214938143157</v>
+        <v>0.44468877391261652</v>
       </c>
       <c r="H40" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I40" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K40" s="2">
         <f t="shared" si="4"/>
@@ -2647,15 +2647,15 @@
       </c>
       <c r="G41" s="19">
         <f t="shared" si="1"/>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="H41" s="19">
         <f t="shared" si="2"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="I41" s="19">
         <f t="shared" si="3"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K41" s="2">
         <f t="shared" si="4"/>
@@ -2688,15 +2688,15 @@
       </c>
       <c r="G42" s="19">
         <f t="shared" si="1"/>
-        <v>0.51490171967079768</v>
+        <v>0.45583905928709567</v>
       </c>
       <c r="H42" s="19">
         <f t="shared" si="2"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="I42" s="19">
         <f t="shared" si="3"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K42" s="2">
         <f t="shared" si="4"/>
@@ -2729,15 +2729,15 @@
       </c>
       <c r="G43" s="19">
         <f t="shared" si="1"/>
-        <v>0.47850906740128607</v>
+        <v>0.42169808713392831</v>
       </c>
       <c r="H43" s="19">
         <f t="shared" si="2"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="I43" s="19">
         <f t="shared" si="3"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K43" s="2">
         <f t="shared" si="4"/>
@@ -2770,15 +2770,15 @@
       </c>
       <c r="G44" s="19">
         <f t="shared" si="1"/>
-        <v>0.49093361615337672</v>
+        <v>0.43331001042692008</v>
       </c>
       <c r="H44" s="19">
         <f t="shared" si="2"/>
-        <v>0.15531728952486967</v>
+        <v>0.1323663538771066</v>
       </c>
       <c r="I44" s="19">
         <f t="shared" si="3"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K44" s="2">
         <f t="shared" si="4"/>
@@ -2811,15 +2811,15 @@
       </c>
       <c r="G45" s="19">
         <f t="shared" si="1"/>
-        <v>0.52645921157860687</v>
+        <v>0.46676545424104743</v>
       </c>
       <c r="H45" s="19">
         <f t="shared" si="2"/>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="I45" s="19">
         <f t="shared" si="3"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" si="4"/>
@@ -2852,15 +2852,15 @@
       </c>
       <c r="G46" s="19">
         <f t="shared" si="1"/>
-        <v>0.52071530159105595</v>
+        <v>0.46132995995618065</v>
       </c>
       <c r="H46" s="19">
         <f t="shared" si="2"/>
-        <v>0.2047333884389867</v>
+        <v>0.17526644285268</v>
       </c>
       <c r="I46" s="19">
         <f t="shared" si="3"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K46" s="2">
         <f t="shared" si="4"/>
@@ -2893,15 +2893,15 @@
       </c>
       <c r="G47" s="19">
         <f t="shared" si="1"/>
-        <v>0.52645921157860687</v>
+        <v>0.46676545424104743</v>
       </c>
       <c r="H47" s="19">
         <f t="shared" si="2"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I47" s="19">
         <f t="shared" si="3"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K47" s="2">
         <f t="shared" si="4"/>
@@ -2934,15 +2934,15 @@
       </c>
       <c r="G48" s="19">
         <f t="shared" si="1"/>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="H48" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I48" s="19">
         <f t="shared" si="3"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K48" s="2">
         <f t="shared" si="4"/>
@@ -2975,15 +2975,15 @@
       </c>
       <c r="G49" s="19">
         <f t="shared" si="1"/>
-        <v>0.50306214938143157</v>
+        <v>0.44468877391261652</v>
       </c>
       <c r="H49" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I49" s="19">
         <f t="shared" si="3"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K49" s="2">
         <f t="shared" si="4"/>
@@ -3016,15 +3016,15 @@
       </c>
       <c r="G50" s="19">
         <f t="shared" si="1"/>
-        <v>0.53213428460546475</v>
+        <v>0.47214610122436662</v>
       </c>
       <c r="H50" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I50" s="19">
         <f t="shared" si="3"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K50" s="2">
         <f t="shared" si="4"/>
@@ -3057,15 +3057,15 @@
       </c>
       <c r="G51" s="19">
         <f t="shared" si="1"/>
-        <v>0.53774134563705722</v>
+        <v>0.47747245434733998</v>
       </c>
       <c r="H51" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I51" s="19">
         <f t="shared" si="3"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="K51" s="2">
         <f t="shared" si="4"/>
@@ -3098,15 +3098,15 @@
       </c>
       <c r="G52" s="19">
         <f t="shared" si="1"/>
-        <v>0.53213428460546475</v>
+        <v>0.47214610122436662</v>
       </c>
       <c r="H52" s="19">
         <f t="shared" si="2"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="I52" s="19">
         <f t="shared" si="3"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="K52" s="2">
         <f t="shared" si="4"/>
@@ -3139,15 +3139,15 @@
       </c>
       <c r="G53" s="19">
         <f t="shared" si="1"/>
-        <v>0.54328120975214667</v>
+        <v>0.48274506146662466</v>
       </c>
       <c r="H53" s="19">
         <f t="shared" si="2"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="I53" s="19">
         <f t="shared" si="3"/>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="K53" s="2">
         <f t="shared" si="4"/>
@@ -3180,15 +3180,15 @@
       </c>
       <c r="G54" s="19">
         <f t="shared" si="1"/>
-        <v>0.53213428460546475</v>
+        <v>0.47214610122436662</v>
       </c>
       <c r="H54" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I54" s="19">
         <f t="shared" si="3"/>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="K54" s="2">
         <f t="shared" si="4"/>
@@ -3221,15 +3221,15 @@
       </c>
       <c r="G55" s="19">
         <f t="shared" si="1"/>
-        <v>0.5541625588240332</v>
+        <v>0.4931312015355781</v>
       </c>
       <c r="H55" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I55" s="19">
         <f t="shared" si="3"/>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="K55" s="2">
         <f t="shared" si="4"/>
@@ -3262,15 +3262,15 @@
       </c>
       <c r="G56" s="19">
         <f t="shared" si="1"/>
-        <v>0.57515368744915019</v>
+        <v>0.51328202850696369</v>
       </c>
       <c r="H56" s="19">
         <f t="shared" si="2"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="I56" s="19">
         <f t="shared" si="3"/>
-        <v>0.18532368255428877</v>
+        <v>0.15836700404317228</v>
       </c>
       <c r="K56" s="2">
         <f t="shared" si="4"/>
@@ -3303,15 +3303,15 @@
       </c>
       <c r="G57" s="19">
         <f t="shared" si="1"/>
-        <v>0.6048019193821581</v>
+        <v>0.54201619718511251</v>
       </c>
       <c r="H57" s="19">
         <f t="shared" si="2"/>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="I57" s="19">
         <f t="shared" si="3"/>
-        <v>0.2047333884389867</v>
+        <v>0.17526644285268</v>
       </c>
       <c r="K57" s="2">
         <f t="shared" si="4"/>
@@ -3344,15 +3344,15 @@
       </c>
       <c r="G58" s="19">
         <f t="shared" si="1"/>
-        <v>0.71114866537895804</v>
+        <v>0.64817072189415192</v>
       </c>
       <c r="H58" s="19">
         <f t="shared" si="2"/>
-        <v>0.45274284813652177</v>
+        <v>0.39775555271787122</v>
       </c>
       <c r="I58" s="19">
         <f t="shared" si="3"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="K58" s="2">
         <f t="shared" si="4"/>
@@ -3385,15 +3385,15 @@
       </c>
       <c r="G59" s="19">
         <f t="shared" si="1"/>
-        <v>0.61421753432852066</v>
+        <v>0.55121221170521451</v>
       </c>
       <c r="H59" s="19">
         <f t="shared" si="2"/>
-        <v>0.3598795970481059</v>
+        <v>0.31288113032139719</v>
       </c>
       <c r="I59" s="19">
         <f t="shared" si="3"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="K59" s="2">
         <f t="shared" si="4"/>
@@ -3426,15 +3426,15 @@
       </c>
       <c r="G60" s="19">
         <f t="shared" si="1"/>
-        <v>0.6048019193821581</v>
+        <v>0.54201619718511251</v>
       </c>
       <c r="H60" s="19">
         <f t="shared" si="2"/>
-        <v>0.3521151255059447</v>
+        <v>0.30587702543196937</v>
       </c>
       <c r="I60" s="19">
         <f t="shared" si="3"/>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="K60" s="2">
         <f t="shared" si="4"/>
@@ -3467,15 +3467,15 @@
       </c>
       <c r="G61" s="19">
         <f t="shared" si="1"/>
-        <v>0.6048019193821581</v>
+        <v>0.54201619718511251</v>
       </c>
       <c r="H61" s="19">
         <f t="shared" si="2"/>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="I61" s="19">
         <f t="shared" si="3"/>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="K61" s="2">
         <f t="shared" si="4"/>
@@ -3508,15 +3508,15 @@
       </c>
       <c r="G62" s="19">
         <f t="shared" si="1"/>
-        <v>0.5541625588240332</v>
+        <v>0.4931312015355781</v>
       </c>
       <c r="H62" s="19">
         <f t="shared" si="2"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="I62" s="19">
         <f t="shared" si="3"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="K62" s="2">
         <f t="shared" si="4"/>
@@ -3549,15 +3549,15 @@
       </c>
       <c r="G63" s="19">
         <f t="shared" si="1"/>
-        <v>0.53213428460546475</v>
+        <v>0.47214610122436662</v>
       </c>
       <c r="H63" s="19">
         <f t="shared" si="2"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="I63" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K63" s="2">
         <f t="shared" si="4"/>
@@ -3590,15 +3590,15 @@
       </c>
       <c r="G64" s="19">
         <f t="shared" si="1"/>
-        <v>0.54328120975214667</v>
+        <v>0.48274506146662466</v>
       </c>
       <c r="H64" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I64" s="19">
         <f t="shared" si="3"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="K64" s="2">
         <f t="shared" si="4"/>
@@ -3631,15 +3631,15 @@
       </c>
       <c r="G65" s="19">
         <f t="shared" si="1"/>
-        <v>0.60953810689212307</v>
+        <v>0.54663752036573587</v>
       </c>
       <c r="H65" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I65" s="19">
         <f t="shared" si="3"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="K65" s="2">
         <f t="shared" si="4"/>
@@ -3672,15 +3672,15 @@
       </c>
       <c r="G66" s="19">
         <f t="shared" si="1"/>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="H66" s="19">
         <f t="shared" si="2"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I66" s="19">
         <f t="shared" si="3"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="K66" s="2">
         <f t="shared" si="4"/>
@@ -3713,15 +3713,15 @@
       </c>
       <c r="G67" s="19">
         <f t="shared" si="1"/>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="H67" s="19">
         <f t="shared" si="2"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I67" s="19">
         <f t="shared" si="3"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="K67" s="2">
         <f t="shared" si="4"/>
@@ -3754,15 +3754,15 @@
       </c>
       <c r="G68" s="19">
         <f t="shared" si="1"/>
-        <v>0.55950562556431493</v>
+        <v>0.4982458027801665</v>
       </c>
       <c r="H68" s="19">
         <f t="shared" si="2"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="I68" s="19">
         <f t="shared" si="3"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K68" s="2">
         <f t="shared" si="4"/>
@@ -3795,15 +3795,15 @@
       </c>
       <c r="G69" s="19">
         <f t="shared" si="1"/>
-        <v>0.5541625588240332</v>
+        <v>0.4931312015355781</v>
       </c>
       <c r="H69" s="19">
         <f t="shared" si="2"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I69" s="19">
         <f t="shared" si="3"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K69" s="2">
         <f t="shared" si="4"/>
@@ -3836,15 +3836,15 @@
       </c>
       <c r="G70" s="19">
         <f t="shared" ref="G70:G133" si="10">(1-(1/(2.71828^((C70*($B$1/100))/141))))</f>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="H70" s="19">
         <f t="shared" ref="H70:H133" si="11">(1-(1/(2.71828^((D70*($B$1/100))/141))))</f>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="I70" s="19">
         <f t="shared" ref="I70:I133" si="12">IF(E70*($B$1/100)&gt;0, (1-(1/(2.71828^(E70*($B$1/100)/141)))), "&lt;1%")</f>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K70" s="2">
         <f t="shared" ref="K70:K132" si="13">(1-(1/(2.71828^(C70/141))))</f>
@@ -3877,15 +3877,15 @@
       </c>
       <c r="G71" s="19">
         <f t="shared" si="10"/>
-        <v>0.58024518940182213</v>
+        <v>0.51819329617682908</v>
       </c>
       <c r="H71" s="19">
         <f t="shared" si="11"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="I71" s="19">
         <f t="shared" si="12"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K71" s="2">
         <f t="shared" si="13"/>
@@ -3918,15 +3918,15 @@
       </c>
       <c r="G72" s="19">
         <f t="shared" si="10"/>
-        <v>0.53774134563705722</v>
+        <v>0.47747245434733998</v>
       </c>
       <c r="H72" s="19">
         <f t="shared" si="11"/>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="I72" s="19">
         <f t="shared" si="12"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K72" s="2">
         <f t="shared" si="13"/>
@@ -3959,15 +3959,15 @@
       </c>
       <c r="G73" s="19">
         <f t="shared" si="10"/>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="H73" s="19">
         <f t="shared" si="11"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="I73" s="19">
         <f t="shared" si="12"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K73" s="2">
         <f t="shared" si="13"/>
@@ -4000,15 +4000,15 @@
       </c>
       <c r="G74" s="19">
         <f t="shared" si="10"/>
-        <v>0.58024518940182213</v>
+        <v>0.51819329617682908</v>
       </c>
       <c r="H74" s="19">
         <f t="shared" si="11"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I74" s="19">
         <f t="shared" si="12"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K74" s="2">
         <f t="shared" si="13"/>
@@ -4041,15 +4041,15 @@
       </c>
       <c r="G75" s="19">
         <f t="shared" si="10"/>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="H75" s="19">
         <f t="shared" si="11"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="I75" s="19">
         <f t="shared" si="12"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="K75" s="2">
         <f t="shared" si="13"/>
@@ -4082,15 +4082,15 @@
       </c>
       <c r="G76" s="19">
         <f t="shared" si="10"/>
-        <v>0.58024518940182213</v>
+        <v>0.51819329617682908</v>
       </c>
       <c r="H76" s="19">
         <f t="shared" si="11"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I76" s="19">
         <f t="shared" si="12"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K76" s="2">
         <f t="shared" si="13"/>
@@ -4123,15 +4123,15 @@
       </c>
       <c r="G77" s="19">
         <f t="shared" si="10"/>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="H77" s="19">
         <f t="shared" si="11"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="I77" s="19">
         <f t="shared" si="12"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="K77" s="2">
         <f t="shared" si="13"/>
@@ -4164,15 +4164,15 @@
       </c>
       <c r="G78" s="19">
         <f t="shared" si="10"/>
-        <v>0.5541625588240332</v>
+        <v>0.4931312015355781</v>
       </c>
       <c r="H78" s="19">
         <f t="shared" si="11"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I78" s="19">
         <f t="shared" si="12"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K78" s="2">
         <f t="shared" si="13"/>
@@ -4205,15 +4205,15 @@
       </c>
       <c r="G79" s="19">
         <f t="shared" si="10"/>
-        <v>0.57515368744915019</v>
+        <v>0.51328202850696369</v>
       </c>
       <c r="H79" s="19">
         <f t="shared" si="11"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I79" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K79" s="2">
         <f t="shared" si="13"/>
@@ -4246,15 +4246,15 @@
       </c>
       <c r="G80" s="19">
         <f t="shared" si="10"/>
-        <v>0.61884088192327691</v>
+        <v>0.55574074174597166</v>
       </c>
       <c r="H80" s="19">
         <f t="shared" si="11"/>
-        <v>0.32825204299627064</v>
+        <v>0.28443341673236711</v>
       </c>
       <c r="I80" s="19">
         <f t="shared" si="12"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="K80" s="2">
         <f t="shared" si="13"/>
@@ -4287,15 +4287,15 @@
       </c>
       <c r="G81" s="19">
         <f t="shared" si="10"/>
-        <v>0.53774134563705722</v>
+        <v>0.47747245434733998</v>
       </c>
       <c r="H81" s="19">
         <f t="shared" si="11"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="I81" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K81" s="2">
         <f t="shared" si="13"/>
@@ -4328,15 +4328,15 @@
       </c>
       <c r="G82" s="19">
         <f t="shared" si="10"/>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="H82" s="19">
         <f t="shared" si="11"/>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="I82" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K82" s="2">
         <f t="shared" si="13"/>
@@ -4369,15 +4369,15 @@
       </c>
       <c r="G83" s="19">
         <f t="shared" si="10"/>
-        <v>0.59024586972470483</v>
+        <v>0.52786765893159926</v>
       </c>
       <c r="H83" s="19">
         <f t="shared" si="11"/>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="I83" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K83" s="2">
         <f t="shared" si="13"/>
@@ -4410,15 +4410,15 @@
       </c>
       <c r="G84" s="19">
         <f t="shared" si="10"/>
-        <v>0.57515368744915019</v>
+        <v>0.51328202850696369</v>
       </c>
       <c r="H84" s="19">
         <f t="shared" si="11"/>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="I84" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K84" s="2">
         <f t="shared" si="13"/>
@@ -4451,15 +4451,15 @@
       </c>
       <c r="G85" s="19">
         <f t="shared" si="10"/>
-        <v>0.60000828331568745</v>
+        <v>0.53734776682447505</v>
       </c>
       <c r="H85" s="19">
         <f t="shared" si="11"/>
-        <v>0.34425647321583208</v>
+        <v>0.2988015246204283</v>
       </c>
       <c r="I85" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K85" s="2">
         <f t="shared" si="13"/>
@@ -4492,15 +4492,15 @@
       </c>
       <c r="G86" s="19">
         <f t="shared" si="10"/>
-        <v>0.59024586972470483</v>
+        <v>0.52786765893159926</v>
       </c>
       <c r="H86" s="19">
         <f t="shared" si="11"/>
-        <v>0.34425647321583208</v>
+        <v>0.2988015246204283</v>
       </c>
       <c r="I86" s="19">
         <f t="shared" si="12"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K86" s="2">
         <f t="shared" si="13"/>
@@ -4533,15 +4533,15 @@
       </c>
       <c r="G87" s="19">
         <f t="shared" si="10"/>
-        <v>0.67018358979238801</v>
+        <v>0.60664745877960757</v>
       </c>
       <c r="H87" s="19">
         <f t="shared" si="11"/>
-        <v>0.425703551980676</v>
+        <v>0.37282176279753421</v>
       </c>
       <c r="I87" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K87" s="2">
         <f t="shared" si="13"/>
@@ -4574,15 +4574,15 @@
       </c>
       <c r="G88" s="19">
         <f t="shared" si="10"/>
-        <v>0.68947869332440015</v>
+        <v>0.62609674949410399</v>
       </c>
       <c r="H88" s="19">
         <f t="shared" si="11"/>
-        <v>0.41873750558245582</v>
+        <v>0.36642865914170353</v>
       </c>
       <c r="I88" s="19">
         <f t="shared" si="12"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="K88" s="2">
         <f t="shared" si="13"/>
@@ -4615,15 +4615,15 @@
       </c>
       <c r="G89" s="19">
         <f t="shared" si="10"/>
-        <v>0.67804148302064327</v>
+        <v>0.61454571993720519</v>
       </c>
       <c r="H89" s="19">
         <f t="shared" si="11"/>
-        <v>0.41873750558245582</v>
+        <v>0.36642865914170353</v>
       </c>
       <c r="I89" s="19">
         <f t="shared" si="12"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="K89" s="2">
         <f t="shared" si="13"/>
@@ -4656,15 +4656,15 @@
       </c>
       <c r="G90" s="19">
         <f t="shared" si="10"/>
-        <v>0.53213428460546475</v>
+        <v>0.47214610122436662</v>
       </c>
       <c r="H90" s="19">
         <f t="shared" si="11"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I90" s="19">
         <f t="shared" si="12"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K90" s="2">
         <f t="shared" si="13"/>
@@ -4697,15 +4697,15 @@
       </c>
       <c r="G91" s="19">
         <f t="shared" si="10"/>
-        <v>0.54875468226131585</v>
+        <v>0.48796446491068579</v>
       </c>
       <c r="H91" s="19">
         <f t="shared" si="11"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="I91" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K91" s="2">
         <f t="shared" si="13"/>
@@ -4738,15 +4738,15 @@
       </c>
       <c r="G92" s="19">
         <f t="shared" si="10"/>
-        <v>0.49703443993558749</v>
+        <v>0.43902824231404158</v>
       </c>
       <c r="H92" s="19">
         <f t="shared" si="11"/>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="I92" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K92" s="2">
         <f t="shared" si="13"/>
@@ -4779,15 +4779,15 @@
       </c>
       <c r="G93" s="19">
         <f t="shared" si="10"/>
-        <v>0.52071530159105595</v>
+        <v>0.46132995995618065</v>
       </c>
       <c r="H93" s="19">
         <f t="shared" si="11"/>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="I93" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K93" s="2">
         <f t="shared" si="13"/>
@@ -4820,15 +4820,15 @@
       </c>
       <c r="G94" s="19">
         <f t="shared" si="10"/>
-        <v>0.4461047804194278</v>
+        <v>0.39161661015060845</v>
       </c>
       <c r="H94" s="19">
         <f t="shared" si="11"/>
-        <v>0.18532368255428877</v>
+        <v>0.15836700404317228</v>
       </c>
       <c r="I94" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K94" s="2">
         <f t="shared" si="13"/>
@@ -4861,15 +4861,15 @@
       </c>
       <c r="G95" s="19">
         <f t="shared" si="10"/>
-        <v>0.60000828331568745</v>
+        <v>0.53734776682447505</v>
       </c>
       <c r="H95" s="19">
         <f t="shared" si="11"/>
-        <v>0.31185700002005889</v>
+        <v>0.26977089502064311</v>
       </c>
       <c r="I95" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K95" s="2">
         <f t="shared" si="13"/>
@@ -4902,11 +4902,11 @@
       </c>
       <c r="G96" s="19">
         <f t="shared" si="10"/>
-        <v>0.39001804768716197</v>
+        <v>0.34019789058285854</v>
       </c>
       <c r="H96" s="19">
         <f t="shared" si="11"/>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="I96" s="19" t="str">
         <f t="shared" si="12"/>
@@ -4943,11 +4943,11 @@
       </c>
       <c r="G97" s="19">
         <f t="shared" si="10"/>
-        <v>0.425703551980676</v>
+        <v>0.37282176279753421</v>
       </c>
       <c r="H97" s="19">
         <f t="shared" si="11"/>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="I97" s="19" t="str">
         <f t="shared" si="12"/>
@@ -4984,15 +4984,15 @@
       </c>
       <c r="G98" s="19">
         <f t="shared" si="10"/>
-        <v>0.585275673072428</v>
+        <v>0.52305500629686519</v>
       </c>
       <c r="H98" s="19">
         <f t="shared" si="11"/>
-        <v>0.31185700002005889</v>
+        <v>0.26977089502064311</v>
       </c>
       <c r="I98" s="19">
         <f t="shared" si="12"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K98" s="2">
         <f t="shared" si="13"/>
@@ -5025,15 +5025,15 @@
       </c>
       <c r="G99" s="19">
         <f t="shared" si="10"/>
-        <v>0.48475879117948029</v>
+        <v>0.42753349008682928</v>
       </c>
       <c r="H99" s="19">
         <f t="shared" si="11"/>
-        <v>0.2047333884389867</v>
+        <v>0.17526644285268</v>
       </c>
       <c r="I99" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K99" s="2">
         <f t="shared" si="13"/>
@@ -5066,15 +5066,15 @@
       </c>
       <c r="G100" s="19">
         <f t="shared" si="10"/>
-        <v>0.46578127841061079</v>
+        <v>0.4098482264059311</v>
       </c>
       <c r="H100" s="19">
         <f t="shared" si="11"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="I100" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K100" s="2">
         <f t="shared" si="13"/>
@@ -5107,15 +5107,15 @@
       </c>
       <c r="G101" s="19">
         <f t="shared" si="10"/>
-        <v>0.53774134563705722</v>
+        <v>0.47747245434733998</v>
       </c>
       <c r="H101" s="19">
         <f t="shared" si="11"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="I101" s="19">
         <f t="shared" si="12"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K101" s="2">
         <f t="shared" si="13"/>
@@ -5148,15 +5148,15 @@
       </c>
       <c r="G102" s="19">
         <f t="shared" si="10"/>
-        <v>0.50306214938143157</v>
+        <v>0.44468877391261652</v>
       </c>
       <c r="H102" s="19">
         <f t="shared" si="11"/>
-        <v>0.2047333884389867</v>
+        <v>0.17526644285268</v>
       </c>
       <c r="I102" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K102" s="2">
         <f t="shared" si="13"/>
@@ -5189,11 +5189,11 @@
       </c>
       <c r="G103" s="19">
         <f t="shared" si="10"/>
-        <v>0.45274284813652177</v>
+        <v>0.39775555271787122</v>
       </c>
       <c r="H103" s="19">
         <f t="shared" si="11"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="I103" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5230,11 +5230,11 @@
       </c>
       <c r="G104" s="19">
         <f t="shared" si="10"/>
-        <v>0.41168696309760733</v>
+        <v>0.35997038776810175</v>
       </c>
       <c r="H104" s="19">
         <f t="shared" si="11"/>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="I104" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5271,11 +5271,11 @@
       </c>
       <c r="G105" s="19">
         <f t="shared" si="10"/>
-        <v>0.41168696309760733</v>
+        <v>0.35997038776810175</v>
       </c>
       <c r="H105" s="19">
         <f t="shared" si="11"/>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="I105" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5312,11 +5312,11 @@
       </c>
       <c r="G106" s="19">
         <f t="shared" si="10"/>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="H106" s="19">
         <f t="shared" si="11"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I106" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5353,11 +5353,11 @@
       </c>
       <c r="G107" s="19">
         <f t="shared" si="10"/>
-        <v>0.31185700002005889</v>
+        <v>0.26977089502064311</v>
       </c>
       <c r="H107" s="19">
         <f t="shared" si="11"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="I107" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5394,11 +5394,11 @@
       </c>
       <c r="G108" s="19">
         <f t="shared" si="10"/>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="H108" s="19">
         <f t="shared" si="11"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I108" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5435,11 +5435,11 @@
       </c>
       <c r="G109" s="19">
         <f t="shared" si="10"/>
-        <v>0.32825204299627064</v>
+        <v>0.28443341673236711</v>
       </c>
       <c r="H109" s="19">
         <f t="shared" si="11"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="I109" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5476,11 +5476,11 @@
       </c>
       <c r="G110" s="19">
         <f t="shared" si="10"/>
-        <v>0.30351002855087539</v>
+        <v>0.26232734853940509</v>
       </c>
       <c r="H110" s="19">
         <f t="shared" si="11"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="I110" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5517,11 +5517,11 @@
       </c>
       <c r="G111" s="19">
         <f t="shared" si="10"/>
-        <v>0.38261914665522456</v>
+        <v>0.3334722374469099</v>
       </c>
       <c r="H111" s="19">
         <f t="shared" si="11"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I111" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5558,11 +5558,11 @@
       </c>
       <c r="G112" s="19">
         <f t="shared" si="10"/>
-        <v>0.41168696309760733</v>
+        <v>0.35997038776810175</v>
       </c>
       <c r="H112" s="19">
         <f t="shared" si="11"/>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="I112" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5599,11 +5599,11 @@
       </c>
       <c r="G113" s="19">
         <f t="shared" si="10"/>
-        <v>0.34425647321583208</v>
+        <v>0.2988015246204283</v>
       </c>
       <c r="H113" s="19">
         <f t="shared" si="11"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="I113" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5640,11 +5640,11 @@
       </c>
       <c r="G114" s="19">
         <f t="shared" si="10"/>
-        <v>0.39732827778577862</v>
+        <v>0.34685567796340067</v>
       </c>
       <c r="H114" s="19">
         <f t="shared" si="11"/>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="I114" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5681,11 +5681,11 @@
       </c>
       <c r="G115" s="19">
         <f t="shared" si="10"/>
-        <v>0.36755101653626432</v>
+        <v>0.31981455971512818</v>
       </c>
       <c r="H115" s="19">
         <f t="shared" si="11"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I115" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5722,11 +5722,11 @@
       </c>
       <c r="G116" s="19">
         <f t="shared" si="10"/>
-        <v>0.36755101653626432</v>
+        <v>0.31981455971512818</v>
       </c>
       <c r="H116" s="19">
         <f t="shared" si="11"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I116" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5763,11 +5763,11 @@
       </c>
       <c r="G117" s="19">
         <f t="shared" si="10"/>
-        <v>0.39001804768716197</v>
+        <v>0.34019789058285854</v>
       </c>
       <c r="H117" s="19">
         <f t="shared" si="11"/>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="I117" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5804,15 +5804,15 @@
       </c>
       <c r="G118" s="19">
         <f t="shared" si="10"/>
-        <v>0.36755101653626432</v>
+        <v>0.31981455971512818</v>
       </c>
       <c r="H118" s="19">
         <f t="shared" si="11"/>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="I118" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K118" s="2">
         <f t="shared" si="13"/>
@@ -5845,11 +5845,11 @@
       </c>
       <c r="G119" s="19">
         <f t="shared" si="10"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="H119" s="19">
         <f t="shared" si="11"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="I119" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5886,11 +5886,11 @@
       </c>
       <c r="G120" s="19">
         <f t="shared" si="10"/>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="H120" s="19">
         <f t="shared" si="11"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="I120" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5927,11 +5927,11 @@
       </c>
       <c r="G121" s="19">
         <f t="shared" si="10"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="H121" s="19">
         <f t="shared" si="11"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="I121" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5968,11 +5968,11 @@
       </c>
       <c r="G122" s="19">
         <f t="shared" si="10"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="H122" s="19">
         <f t="shared" si="11"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="I122" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6009,11 +6009,11 @@
       </c>
       <c r="G123" s="19">
         <f t="shared" si="10"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="H123" s="19">
         <f t="shared" si="11"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="I123" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6050,7 +6050,7 @@
       </c>
       <c r="G124" s="19">
         <f t="shared" si="10"/>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="H124" s="19">
         <f t="shared" si="11"/>
@@ -6091,7 +6091,7 @@
       </c>
       <c r="G125" s="19">
         <f t="shared" si="10"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="H125" s="19">
         <f t="shared" si="11"/>
@@ -6132,11 +6132,11 @@
       </c>
       <c r="G126" s="19">
         <f t="shared" si="10"/>
-        <v>0.2047333884389867</v>
+        <v>0.17526644285268</v>
       </c>
       <c r="H126" s="19">
         <f t="shared" si="11"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="I126" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6173,11 +6173,11 @@
       </c>
       <c r="G127" s="19">
         <f t="shared" si="10"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="H127" s="19">
         <f t="shared" si="11"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="I127" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6214,11 +6214,11 @@
       </c>
       <c r="G128" s="19">
         <f t="shared" si="10"/>
-        <v>0.32825204299627064</v>
+        <v>0.28443341673236711</v>
       </c>
       <c r="H128" s="19">
         <f t="shared" si="11"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I128" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6255,11 +6255,11 @@
       </c>
       <c r="G129" s="19">
         <f t="shared" si="10"/>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="H129" s="19">
         <f t="shared" si="11"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="I129" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6296,11 +6296,11 @@
       </c>
       <c r="G130" s="19">
         <f t="shared" si="10"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="H130" s="19">
         <f t="shared" si="11"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="I130" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6337,11 +6337,11 @@
       </c>
       <c r="G131" s="19">
         <f t="shared" si="10"/>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="H131" s="19">
         <f t="shared" si="11"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="I131" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6378,15 +6378,15 @@
       </c>
       <c r="G132" s="19">
         <f t="shared" si="10"/>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="H132" s="19">
         <f t="shared" si="11"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I132" s="19">
         <f t="shared" si="12"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K132" s="2">
         <f t="shared" si="13"/>
@@ -6419,11 +6419,11 @@
       </c>
       <c r="G133" s="19">
         <f t="shared" si="10"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H133" s="19">
         <f t="shared" si="11"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="I133" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6460,11 +6460,11 @@
       </c>
       <c r="G134" s="19">
         <f t="shared" ref="G134:G177" si="19">(1-(1/(2.71828^((C134*($B$1/100))/141))))</f>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="H134" s="19">
         <f t="shared" ref="H134:H177" si="20">(1-(1/(2.71828^((D134*($B$1/100))/141))))</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="I134" s="19" t="str">
         <f t="shared" ref="I134:I177" si="21">IF(E134*($B$1/100)&gt;0, (1-(1/(2.71828^(E134*($B$1/100)/141)))), "&lt;1%")</f>
@@ -6501,15 +6501,15 @@
       </c>
       <c r="G135" s="19">
         <f t="shared" si="19"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="H135" s="19">
         <f t="shared" si="20"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I135" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K135" s="2">
         <f t="shared" si="16"/>
@@ -6542,15 +6542,15 @@
       </c>
       <c r="G136" s="19">
         <f t="shared" si="19"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="H136" s="19">
         <f t="shared" si="20"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I136" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K136" s="2">
         <f t="shared" si="16"/>
@@ -6583,15 +6583,15 @@
       </c>
       <c r="G137" s="19">
         <f t="shared" si="19"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="H137" s="19">
         <f t="shared" si="20"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I137" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K137" s="2">
         <f t="shared" si="16"/>
@@ -6624,15 +6624,15 @@
       </c>
       <c r="G138" s="19">
         <f t="shared" si="19"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="H138" s="19">
         <f t="shared" si="20"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I138" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K138" s="2">
         <f t="shared" si="16"/>
@@ -6665,11 +6665,11 @@
       </c>
       <c r="G139" s="19">
         <f t="shared" si="19"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="H139" s="19">
         <f t="shared" si="20"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="I139" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6706,11 +6706,11 @@
       </c>
       <c r="G140" s="19">
         <f t="shared" si="19"/>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="H140" s="19">
         <f t="shared" si="20"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="I140" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6747,11 +6747,11 @@
       </c>
       <c r="G141" s="19">
         <f t="shared" si="19"/>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="H141" s="19">
         <f t="shared" si="20"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="I141" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6788,11 +6788,11 @@
       </c>
       <c r="G142" s="19">
         <f t="shared" si="19"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="H142" s="19">
         <f t="shared" si="20"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="I142" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6829,11 +6829,11 @@
       </c>
       <c r="G143" s="19">
         <f t="shared" si="19"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="H143" s="19">
         <f t="shared" si="20"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="I143" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6870,11 +6870,11 @@
       </c>
       <c r="G144" s="19">
         <f t="shared" si="19"/>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="H144" s="19">
         <f t="shared" si="20"/>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="I144" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6911,11 +6911,11 @@
       </c>
       <c r="G145" s="19">
         <f t="shared" si="19"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="H145" s="19">
         <f t="shared" si="20"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="I145" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6952,15 +6952,15 @@
       </c>
       <c r="G146" s="19">
         <f t="shared" si="19"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="H146" s="19">
         <f t="shared" si="20"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="I146" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K146" s="2">
         <f t="shared" si="16"/>
@@ -6993,15 +6993,15 @@
       </c>
       <c r="G147" s="19">
         <f t="shared" si="19"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="H147" s="19">
         <f t="shared" si="20"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="I147" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K147" s="2">
         <f t="shared" si="16"/>
@@ -7034,15 +7034,15 @@
       </c>
       <c r="G148" s="19">
         <f t="shared" si="19"/>
-        <v>0.32825204299627064</v>
+        <v>0.28443341673236711</v>
       </c>
       <c r="H148" s="19">
         <f t="shared" si="20"/>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="I148" s="19">
         <f t="shared" si="21"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="K148" s="2">
         <f t="shared" si="16"/>
@@ -7075,15 +7075,15 @@
       </c>
       <c r="G149" s="19">
         <f t="shared" si="19"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H149" s="19">
         <f t="shared" si="20"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I149" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K149" s="2">
         <f t="shared" si="16"/>
@@ -7116,15 +7116,15 @@
       </c>
       <c r="G150" s="19">
         <f t="shared" si="19"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="H150" s="19">
         <f t="shared" si="20"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I150" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K150" s="2">
         <f t="shared" si="16"/>
@@ -7157,11 +7157,11 @@
       </c>
       <c r="G151" s="19">
         <f t="shared" si="19"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H151" s="19">
         <f t="shared" si="20"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I151" s="19" t="str">
         <f t="shared" si="21"/>
@@ -7198,15 +7198,15 @@
       </c>
       <c r="G152" s="19">
         <f t="shared" si="19"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="H152" s="19">
         <f t="shared" si="20"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I152" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K152" s="2">
         <f t="shared" si="16"/>
@@ -7239,15 +7239,15 @@
       </c>
       <c r="G153" s="19">
         <f t="shared" si="19"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="H153" s="19">
         <f t="shared" si="20"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I153" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K153" s="2">
         <f t="shared" si="16"/>
@@ -7280,15 +7280,15 @@
       </c>
       <c r="G154" s="19">
         <f t="shared" si="19"/>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="H154" s="19">
         <f t="shared" si="20"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I154" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K154" s="2">
         <f t="shared" si="16"/>
@@ -7321,15 +7321,15 @@
       </c>
       <c r="G155" s="19">
         <f t="shared" si="19"/>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="H155" s="19">
         <f t="shared" si="20"/>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="I155" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K155" s="2">
         <f t="shared" si="16"/>
@@ -7362,15 +7362,15 @@
       </c>
       <c r="G156" s="19">
         <f t="shared" si="19"/>
-        <v>0.27785670909526972</v>
+        <v>0.23953835542739466</v>
       </c>
       <c r="H156" s="19">
         <f t="shared" si="20"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I156" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K156" s="2">
         <f t="shared" si="16"/>
@@ -7403,15 +7403,15 @@
       </c>
       <c r="G157" s="19">
         <f t="shared" si="19"/>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="H157" s="19">
         <f t="shared" si="20"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I157" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K157" s="2">
         <f t="shared" si="16"/>
@@ -7444,15 +7444,15 @@
       </c>
       <c r="G158" s="19">
         <f t="shared" si="19"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="H158" s="19">
         <f t="shared" si="20"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I158" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K158" s="2">
         <f t="shared" si="16"/>
@@ -7485,15 +7485,15 @@
       </c>
       <c r="G159" s="19">
         <f t="shared" si="19"/>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="H159" s="19">
         <f t="shared" si="20"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="I159" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K159" s="2">
         <f t="shared" si="16"/>
@@ -7526,15 +7526,15 @@
       </c>
       <c r="G160" s="19">
         <f t="shared" si="19"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H160" s="19">
         <f t="shared" si="20"/>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="I160" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K160" s="2">
         <f t="shared" si="16"/>
@@ -7567,15 +7567,15 @@
       </c>
       <c r="G161" s="19">
         <f t="shared" si="19"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="H161" s="19">
         <f t="shared" si="20"/>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="I161" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K161" s="2">
         <f t="shared" si="16"/>
@@ -7608,15 +7608,15 @@
       </c>
       <c r="G162" s="19">
         <f t="shared" si="19"/>
-        <v>0.31185700002005889</v>
+        <v>0.26977089502064311</v>
       </c>
       <c r="H162" s="19">
         <f t="shared" si="20"/>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="I162" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K162" s="2">
         <f t="shared" si="16"/>
@@ -7649,15 +7649,15 @@
       </c>
       <c r="G163" s="19">
         <f t="shared" si="19"/>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H163" s="19">
         <f t="shared" si="20"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I163" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K163" s="2">
         <f t="shared" si="16"/>
@@ -7690,15 +7690,15 @@
       </c>
       <c r="G164" s="19">
         <f t="shared" si="19"/>
-        <v>0.30351002855087539</v>
+        <v>0.26232734853940509</v>
       </c>
       <c r="H164" s="19">
         <f t="shared" si="20"/>
-        <v>0.15531728952486967</v>
+        <v>0.1323663538771066</v>
       </c>
       <c r="I164" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K164" s="2">
         <f t="shared" si="16"/>
@@ -7731,15 +7731,15 @@
       </c>
       <c r="G165" s="19">
         <f t="shared" si="19"/>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="H165" s="19">
         <f t="shared" si="20"/>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="I165" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K165" s="2">
         <f t="shared" si="16"/>
@@ -7772,15 +7772,15 @@
       </c>
       <c r="G166" s="19">
         <f t="shared" si="19"/>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="H166" s="19">
         <f t="shared" si="20"/>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="I166" s="19">
         <f t="shared" si="21"/>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="K166" s="2">
         <f t="shared" si="16"/>
@@ -7813,15 +7813,15 @@
       </c>
       <c r="G167" s="19">
         <f t="shared" si="19"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="H167" s="19">
         <f t="shared" si="20"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I167" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K167" s="2">
         <f t="shared" si="16"/>
@@ -7854,15 +7854,15 @@
       </c>
       <c r="G168" s="19">
         <f t="shared" si="19"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="H168" s="19">
         <f t="shared" si="20"/>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="I168" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K168" s="2">
         <f t="shared" si="16"/>
@@ -7895,15 +7895,15 @@
       </c>
       <c r="G169" s="19">
         <f t="shared" si="19"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="H169" s="19">
         <f t="shared" si="20"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="I169" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K169" s="2">
         <f t="shared" si="16"/>
@@ -7936,15 +7936,15 @@
       </c>
       <c r="G170" s="19">
         <f t="shared" si="19"/>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="H170" s="19">
         <f t="shared" si="20"/>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="I170" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K170" s="2">
         <f t="shared" si="16"/>
@@ -7977,11 +7977,11 @@
       </c>
       <c r="G171" s="19">
         <f t="shared" si="19"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="H171" s="19">
         <f t="shared" si="20"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="I171" s="19" t="str">
         <f t="shared" si="21"/>
@@ -8018,11 +8018,11 @@
       </c>
       <c r="G172" s="19">
         <f t="shared" si="19"/>
-        <v>0.18532368255428877</v>
+        <v>0.15836700404317228</v>
       </c>
       <c r="H172" s="19">
         <f t="shared" si="20"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="I172" s="19" t="str">
         <f t="shared" si="21"/>
@@ -8059,11 +8059,11 @@
       </c>
       <c r="G173" s="19">
         <f t="shared" si="19"/>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="H173" s="19">
         <f t="shared" si="20"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="I173" s="19" t="str">
         <f t="shared" si="21"/>
@@ -8100,15 +8100,15 @@
       </c>
       <c r="G174" s="19">
         <f t="shared" si="19"/>
-        <v>0.21426413258348997</v>
+        <v>0.18358848455384336</v>
       </c>
       <c r="H174" s="19">
         <f t="shared" si="20"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="I174" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K174" s="2">
         <f t="shared" si="16"/>
@@ -8141,15 +8141,15 @@
       </c>
       <c r="G175" s="19">
         <f t="shared" si="19"/>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="H175" s="19">
         <f t="shared" si="20"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="I175" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K175" s="2">
         <f t="shared" si="16"/>
@@ -8182,15 +8182,15 @@
       </c>
       <c r="G176" s="19">
         <f t="shared" si="19"/>
-        <v>0.19508703918121972</v>
+        <v>0.16685957091974546</v>
       </c>
       <c r="H176" s="19">
         <f t="shared" si="20"/>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="I176" s="19">
         <f t="shared" si="21"/>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="K176" s="2">
         <f t="shared" si="16"/>
@@ -8223,11 +8223,11 @@
       </c>
       <c r="G177" s="19">
         <f t="shared" si="19"/>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="H177" s="19">
         <f t="shared" si="20"/>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="I177" s="19" t="str">
         <f t="shared" si="21"/>
@@ -11025,15 +11025,15 @@
       </c>
       <c r="F4" s="2">
         <f>(1-(1/(2.71828^((B4*(County!$B$1/100))/141))))</f>
-        <v>0.79881794219674895</v>
+        <v>0.74046516355819192</v>
       </c>
       <c r="G4" s="2">
         <f>(1-(1/(2.71828^((C4*(County!$B$1/100))/141))))</f>
-        <v>0.53774134563705722</v>
+        <v>0.47747245434733998</v>
       </c>
       <c r="H4" s="2">
         <f>IF(D4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="J4" s="2">
         <f>(1-(1/(2.71828^(B4/141))))</f>
@@ -11063,15 +11063,15 @@
       </c>
       <c r="F5" s="2">
         <f>(1-(1/(2.71828^((B5*(County!$B$1/100))/141))))</f>
-        <v>0.83806595418997021</v>
+        <v>0.78377103500559842</v>
       </c>
       <c r="G5" s="2">
         <f>(1-(1/(2.71828^((C5*(County!$B$1/100))/141))))</f>
-        <v>0.55950562556431493</v>
+        <v>0.4982458027801665</v>
       </c>
       <c r="H5" s="2">
         <f>IF(D5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ref="J5:J21" si="0">(1-(1/(2.71828^(B5/141))))</f>
@@ -11101,15 +11101,15 @@
       </c>
       <c r="F6" s="2">
         <f>(1-(1/(2.71828^((B6*(County!$B$1/100))/141))))</f>
-        <v>0.72140978066665684</v>
+        <v>0.65871410044924505</v>
       </c>
       <c r="G6" s="2">
         <f>(1-(1/(2.71828^((C6*(County!$B$1/100))/141))))</f>
-        <v>0.43258611492195864</v>
+        <v>0.37915035631580263</v>
       </c>
       <c r="H6" s="2">
         <f>IF(D6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
@@ -11139,15 +11139,15 @@
       </c>
       <c r="F7" s="2">
         <f>(1-(1/(2.71828^((B7*(County!$B$1/100))/141))))</f>
-        <v>0.77303914603711887</v>
+        <v>0.71276252588327726</v>
       </c>
       <c r="G7" s="2">
         <f>(1-(1/(2.71828^((C7*(County!$B$1/100))/141))))</f>
-        <v>0.425703551980676</v>
+        <v>0.37282176279753421</v>
       </c>
       <c r="H7" s="2">
         <f>IF(D7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
@@ -11177,15 +11177,15 @@
       </c>
       <c r="F8" s="2">
         <f>(1-(1/(2.71828^((B8*(County!$B$1/100))/141))))</f>
-        <v>0.9632473106772913</v>
+        <v>0.93789093826413483</v>
       </c>
       <c r="G8" s="2">
         <f>(1-(1/(2.71828^((C8*(County!$B$1/100))/141))))</f>
-        <v>0.75005737564642649</v>
+        <v>0.6884860854390159</v>
       </c>
       <c r="H8" s="2">
         <f>IF(D8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.43938619490029751</v>
+        <v>0.38541509064135093</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
@@ -11215,15 +11215,15 @@
       </c>
       <c r="F9" s="2">
         <f>(1-(1/(2.71828^((B9*(County!$B$1/100))/141))))</f>
-        <v>0.81510036728918622</v>
+        <v>0.75825146410807087</v>
       </c>
       <c r="G9" s="2">
         <f>(1-(1/(2.71828^((C9*(County!$B$1/100))/141))))</f>
-        <v>0.45930136300416158</v>
+        <v>0.40383254978091254</v>
       </c>
       <c r="H9" s="2">
         <f>IF(D9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
@@ -11253,15 +11253,15 @@
       </c>
       <c r="F10" s="2">
         <f>(1-(1/(2.71828^((B10*(County!$B$1/100))/141))))</f>
-        <v>0.7589363032344425</v>
+        <v>0.69782132082385306</v>
       </c>
       <c r="G10" s="2">
         <f>(1-(1/(2.71828^((C10*(County!$B$1/100))/141))))</f>
-        <v>0.43938619490029751</v>
+        <v>0.38541509064135093</v>
       </c>
       <c r="H10" s="2">
         <f>IF(D10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
@@ -11291,15 +11291,15 @@
       </c>
       <c r="F11" s="2">
         <f>(1-(1/(2.71828^((B11*(County!$B$1/100))/141))))</f>
-        <v>0.85295549561519524</v>
+        <v>0.80062187005869268</v>
       </c>
       <c r="G11" s="2">
         <f>(1-(1/(2.71828^((C11*(County!$B$1/100))/141))))</f>
-        <v>0.55950562556431493</v>
+        <v>0.4982458027801665</v>
       </c>
       <c r="H11" s="2">
         <f>IF(D11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D11*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
@@ -11329,15 +11329,15 @@
       </c>
       <c r="F12" s="2">
         <f>(1-(1/(2.71828^((B12*(County!$B$1/100))/141))))</f>
-        <v>0.64544036884895628</v>
+        <v>0.58196829283544926</v>
       </c>
       <c r="G12" s="2">
         <f>(1-(1/(2.71828^((C12*(County!$B$1/100))/141))))</f>
-        <v>0.31185700002005889</v>
+        <v>0.26977089502064311</v>
       </c>
       <c r="H12" s="2">
         <f>IF(D12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D12*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
@@ -11367,15 +11367,15 @@
       </c>
       <c r="F13" s="2">
         <f>(1-(1/(2.71828^((B13*(County!$B$1/100))/141))))</f>
-        <v>0.46578127841061079</v>
+        <v>0.4098482264059311</v>
       </c>
       <c r="G13" s="2">
         <f>(1-(1/(2.71828^((C13*(County!$B$1/100))/141))))</f>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="H13" s="2">
         <f>IF(D13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
@@ -11405,15 +11405,15 @@
       </c>
       <c r="F14" s="2">
         <f>(1-(1/(2.71828^((B14*(County!$B$1/100))/141))))</f>
-        <v>0.3521151255059447</v>
+        <v>0.30587702543196937</v>
       </c>
       <c r="G14" s="2">
         <f>(1-(1/(2.71828^((C14*(County!$B$1/100))/141))))</f>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="H14" s="2">
         <f>IF(D14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
@@ -11443,15 +11443,15 @@
       </c>
       <c r="F15" s="2">
         <f>(1-(1/(2.71828^((B15*(County!$B$1/100))/141))))</f>
-        <v>0.3521151255059447</v>
+        <v>0.30587702543196937</v>
       </c>
       <c r="G15" s="2">
         <f>(1-(1/(2.71828^((C15*(County!$B$1/100))/141))))</f>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="H15" s="2">
         <f>IF(D15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
@@ -11481,15 +11481,15 @@
       </c>
       <c r="F16" s="2">
         <f>(1-(1/(2.71828^((B16*(County!$B$1/100))/141))))</f>
-        <v>0.40455089961354063</v>
+        <v>0.35344628439351555</v>
       </c>
       <c r="G16" s="2">
         <f>(1-(1/(2.71828^((C16*(County!$B$1/100))/141))))</f>
-        <v>0.15531728952486967</v>
+        <v>0.1323663538771066</v>
       </c>
       <c r="H16" s="2">
         <f>IF(D16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D16*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
@@ -11519,15 +11519,15 @@
       </c>
       <c r="F17" s="2">
         <f>(1-(1/(2.71828^((B17*(County!$B$1/100))/141))))</f>
-        <v>0.34425647321583208</v>
+        <v>0.2988015246204283</v>
       </c>
       <c r="G17" s="2">
         <f>(1-(1/(2.71828^((C17*(County!$B$1/100))/141))))</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="H17" s="2">
         <f>IF(D17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
@@ -11557,15 +11557,15 @@
       </c>
       <c r="F18" s="2">
         <f>(1-(1/(2.71828^((B18*(County!$B$1/100))/141))))</f>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="G18" s="2">
         <f>(1-(1/(2.71828^((C18*(County!$B$1/100))/141))))</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="H18" s="2">
         <f>IF(D18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
@@ -11595,15 +11595,15 @@
       </c>
       <c r="F19" s="2">
         <f>(1-(1/(2.71828^((B19*(County!$B$1/100))/141))))</f>
-        <v>0.49093361615337672</v>
+        <v>0.43331001042692008</v>
       </c>
       <c r="G19" s="2">
         <f>(1-(1/(2.71828^((C19*(County!$B$1/100))/141))))</f>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="H19" s="2">
         <f>IF(D19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
@@ -11633,15 +11633,15 @@
       </c>
       <c r="F20" s="2">
         <f>(1-(1/(2.71828^((B20*(County!$B$1/100))/141))))</f>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="G20" s="2">
         <f>(1-(1/(2.71828^((C20*(County!$B$1/100))/141))))</f>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="H20" s="2">
         <f>IF(D20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="0"/>
@@ -11671,15 +11671,15 @@
       </c>
       <c r="F21" s="2">
         <f>(1-(1/(2.71828^((B21*(County!$B$1/100))/141))))</f>
-        <v>0.33630249779309462</v>
+        <v>0.2916539001167342</v>
       </c>
       <c r="G21" s="2">
         <f>(1-(1/(2.71828^((C21*(County!$B$1/100))/141))))</f>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="H21" s="2">
         <f>IF(D21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
@@ -12790,15 +12790,15 @@
       </c>
       <c r="F4" s="3">
         <f>IF(B4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.49703443993558749</v>
+        <v>0.43902824231404158</v>
       </c>
       <c r="G4" s="3">
         <f>IF(C4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="H4" s="3">
         <f>IF(D4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J4" s="3">
         <f>(1-(1/(2.71828^(B4/141))))</f>
@@ -12828,15 +12828,15 @@
       </c>
       <c r="F5" s="3">
         <f>IF(B5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.6048019193821581</v>
+        <v>0.54201619718511251</v>
       </c>
       <c r="G5" s="3">
         <f>IF(C5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.41168696309760733</v>
+        <v>0.35997038776810175</v>
       </c>
       <c r="H5" s="3">
         <f>IF(D5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:K7" si="0">(1-(1/(2.71828^(B5/141))))</f>
@@ -12866,11 +12866,11 @@
       </c>
       <c r="F6" s="3">
         <f>IF(B6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.15531728952486967</v>
+        <v>0.1323663538771066</v>
       </c>
       <c r="G6" s="3">
         <f>IF(C6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="H6" s="3" t="str">
         <f>IF(D6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D6*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -12904,15 +12904,15 @@
       </c>
       <c r="F7" s="3">
         <f>IF(B7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.40455089961354063</v>
+        <v>0.35344628439351555</v>
       </c>
       <c r="G7" s="3">
         <f>IF(C7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.2512585191805502</v>
+        <v>0.21604533973025641</v>
       </c>
       <c r="H7" s="3">
         <f>IF(D7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
@@ -14019,15 +14019,15 @@
       </c>
       <c r="F4" s="3">
         <f>IF(B4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.52071530159105595</v>
+        <v>0.46132995995618065</v>
       </c>
       <c r="G4" s="3">
         <f>IF(C4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="H4" s="3">
         <f>IF(D4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="J4" s="3">
         <f>(1-(1/(2.71828^(B4/141))))</f>
@@ -14057,15 +14057,15 @@
       </c>
       <c r="F5" s="3">
         <f>IF(B5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.425703551980676</v>
+        <v>0.37282176279753421</v>
       </c>
       <c r="G5" s="3">
         <f>IF(C5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H5" s="3">
         <f>IF(D5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:K7" si="0">(1-(1/(2.71828^(B5/141))))</f>
@@ -14095,11 +14095,11 @@
       </c>
       <c r="F6" s="3">
         <f>IF(B6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="G6" s="3">
         <f>IF(C6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>8.0933783411047955E-2</v>
+        <v>6.8531457255322281E-2</v>
       </c>
       <c r="H6" s="3" t="str">
         <f>IF(D6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D6*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14133,15 +14133,15 @@
       </c>
       <c r="F7" s="3">
         <f>IF(B7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.94258472444679964</v>
+        <v>0.90960943662496641</v>
       </c>
       <c r="G7" s="3">
         <f>IF(C7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.72140978066665684</v>
+        <v>0.65871410044924505</v>
       </c>
       <c r="H7" s="3">
         <f>IF(D7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.45274284813652177</v>
+        <v>0.39775555271787122</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
@@ -14171,15 +14171,15 @@
       </c>
       <c r="F8" s="3">
         <f>IF(B8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.43258611492195864</v>
+        <v>0.37915035631580263</v>
       </c>
       <c r="G8" s="3">
         <f>IF(C8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="H8" s="3">
         <f>IF(D8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ref="J8:J41" si="2">(1-(1/(2.71828^(B8/141))))</f>
@@ -14209,15 +14209,15 @@
       </c>
       <c r="F9" s="3">
         <f>IF(B9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.60000828331568745</v>
+        <v>0.53734776682447505</v>
       </c>
       <c r="G9" s="3">
         <f>IF(C9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.30351002855087539</v>
+        <v>0.26232734853940509</v>
       </c>
       <c r="H9" s="3">
         <f>IF(D9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="2"/>
@@ -14247,15 +14247,15 @@
       </c>
       <c r="F10" s="3">
         <f>IF(B10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.57515368744915019</v>
+        <v>0.51328202850696369</v>
       </c>
       <c r="G10" s="3">
         <f>IF(C10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.39732827778577862</v>
+        <v>0.34685567796340067</v>
       </c>
       <c r="H10" s="3">
         <f>IF(D10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.18532368255428877</v>
+        <v>0.15836700404317228</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="2"/>
@@ -14285,11 +14285,11 @@
       </c>
       <c r="F11" s="3">
         <f>IF(B11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B11*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="G11" s="3">
         <f>IF(C11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C11*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="H11" s="3" t="str">
         <f>IF(D11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D11*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14323,11 +14323,11 @@
       </c>
       <c r="F12" s="3">
         <f>IF(B12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B12*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="G12" s="3">
         <f>IF(C12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C12*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="H12" s="3" t="str">
         <f>IF(D12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D12*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14361,15 +14361,15 @@
       </c>
       <c r="F13" s="3">
         <f>IF(B13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.57515368744915019</v>
+        <v>0.51328202850696369</v>
       </c>
       <c r="G13" s="3">
         <f>IF(C13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.3598795970481059</v>
+        <v>0.31288113032139719</v>
       </c>
       <c r="H13" s="3">
         <f>IF(D13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="2"/>
@@ -14399,15 +14399,15 @@
       </c>
       <c r="F14" s="3">
         <f>IF(B14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="G14" s="3">
         <f>IF(C14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="H14" s="3">
         <f>IF(D14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="2"/>
@@ -14437,15 +14437,15 @@
       </c>
       <c r="F15" s="3">
         <f>IF(B15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.91452854459089683</v>
+        <v>0.87367973087526618</v>
       </c>
       <c r="G15" s="3">
         <f>IF(C15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.70764498395084252</v>
+        <v>0.64458437129927193</v>
       </c>
       <c r="H15" s="3">
         <f>IF(D15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.39001804768716197</v>
+        <v>0.34019789058285854</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="2"/>
@@ -14475,11 +14475,11 @@
       </c>
       <c r="F16" s="3">
         <f>IF(B16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B16*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="G16" s="3">
         <f>IF(C16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C16*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="H16" s="3" t="str">
         <f>IF(D16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D16*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14513,15 +14513,15 @@
       </c>
       <c r="F17" s="3">
         <f>IF(B17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.49703443993558749</v>
+        <v>0.43902824231404158</v>
       </c>
       <c r="G17" s="3">
         <f>IF(C17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.22368065706552087</v>
+        <v>0.19182655200965715</v>
       </c>
       <c r="H17" s="3">
         <f>IF(D17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="2"/>
@@ -14551,15 +14551,15 @@
       </c>
       <c r="F18" s="3">
         <f>IF(B18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.77303914603711887</v>
+        <v>0.71276252588327726</v>
       </c>
       <c r="G18" s="3">
         <f>IF(C18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.52071530159105595</v>
+        <v>0.46132995995618065</v>
       </c>
       <c r="H18" s="3">
         <f>IF(D18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.26909732413310372</v>
+        <v>0.23178663537135147</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="2"/>
@@ -14589,15 +14589,15 @@
       </c>
       <c r="F19" s="3">
         <f>IF(B19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.425703551980676</v>
+        <v>0.37282176279753421</v>
       </c>
       <c r="G19" s="3">
         <f>IF(C19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="H19" s="3">
         <f>IF(D19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" si="2"/>
@@ -14627,15 +14627,15 @@
       </c>
       <c r="F20" s="3">
         <f>IF(B20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="G20" s="3">
         <f>IF(C20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.28651111862438716</v>
+        <v>0.2472118561154939</v>
       </c>
       <c r="H20" s="3">
         <f>IF(D20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11358256593379767</v>
+        <v>9.6445067831425813E-2</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" si="2"/>
@@ -14665,15 +14665,15 @@
       </c>
       <c r="F21" s="3">
         <f>IF(B21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.55950562556431493</v>
+        <v>0.4982458027801665</v>
       </c>
       <c r="G21" s="3">
         <f>IF(C21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H21" s="3">
         <f>IF(D21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>4.7082471516410873E-2</v>
+        <v>3.9755508787349569E-2</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" si="2"/>
@@ -14703,15 +14703,15 @@
       </c>
       <c r="F22" s="3">
         <f>IF(B22*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B22*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.62792201785261859</v>
+        <v>0.56466117640869062</v>
       </c>
       <c r="G22" s="3">
         <f>IF(C22*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C22*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.39732827778577862</v>
+        <v>0.34685567796340067</v>
       </c>
       <c r="H22" s="3">
         <f>IF(D22*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D22*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.15531728952486967</v>
+        <v>0.1323663538771066</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" si="2"/>
@@ -14741,15 +14741,15 @@
       </c>
       <c r="F23" s="3">
         <f>IF(B23*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B23*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.82800373265447247</v>
+        <v>0.77252347298151669</v>
       </c>
       <c r="G23" s="3">
         <f>IF(C23*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C23*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.425703551980676</v>
+        <v>0.37282176279753421</v>
       </c>
       <c r="H23" s="3">
         <f>IF(D23*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D23*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" si="2"/>
@@ -14779,15 +14779,15 @@
       </c>
       <c r="F24" s="3">
         <f>IF(B24*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B24*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.65388777061068404</v>
+        <v>0.59036209546628593</v>
       </c>
       <c r="G24" s="3">
         <f>IF(C24*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C24*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.3521151255059447</v>
+        <v>0.30587702543196937</v>
       </c>
       <c r="H24" s="3">
         <f>IF(D24*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D24*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="2"/>
@@ -14817,15 +14817,15 @@
       </c>
       <c r="F25" s="3">
         <f>IF(B25*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B25*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="G25" s="3">
         <f>IF(C25*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C25*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.18532368255428877</v>
+        <v>0.15836700404317228</v>
       </c>
       <c r="H25" s="3">
         <f>IF(D25*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D25*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>6.9785781486474296E-2</v>
+        <v>5.9036588663461731E-2</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" si="2"/>
@@ -14855,15 +14855,15 @@
       </c>
       <c r="F26" s="3">
         <f>IF(B26*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B26*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.91452854459089683</v>
+        <v>0.87367973087526618</v>
       </c>
       <c r="G26" s="3">
         <f>IF(C26*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C26*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.63238112628002896</v>
+        <v>0.56905399856642302</v>
       </c>
       <c r="H26" s="3">
         <f>IF(D26*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D26*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.29506181078156346</v>
+        <v>0.25480792671460639</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" si="2"/>
@@ -14893,15 +14893,15 @@
       </c>
       <c r="F27" s="3">
         <f>IF(B27*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B27*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.40455089961354063</v>
+        <v>0.35344628439351555</v>
       </c>
       <c r="G27" s="3">
         <f>IF(C27*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C27*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.23298433073215996</v>
+        <v>0.19998149256914177</v>
       </c>
       <c r="H27" s="3">
         <f>IF(D27*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D27*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>9.1948183908728165E-2</v>
+        <v>7.7930517095758045E-2</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="2"/>
@@ -14931,15 +14931,15 @@
       </c>
       <c r="F28" s="3">
         <f>IF(B28*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B28*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.52645921157860687</v>
+        <v>0.46676545424104743</v>
       </c>
       <c r="G28" s="3">
         <f>IF(C28*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C28*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.26023169041687233</v>
+        <v>0.22395589862293985</v>
       </c>
       <c r="H28" s="3">
         <f>IF(D28*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D28*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="2"/>
@@ -14969,11 +14969,11 @@
       </c>
       <c r="F29" s="3">
         <f>IF(B29*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B29*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="G29" s="3">
         <f>IF(C29*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C29*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.1984338341321177E-2</v>
+        <v>1.009058213897418E-2</v>
       </c>
       <c r="H29" s="3" t="str">
         <f>IF(D29*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D29*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -15007,15 +15007,15 @@
       </c>
       <c r="F30" s="3">
         <f>IF(B30*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B30*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.585275673072428</v>
+        <v>0.52305500629686519</v>
       </c>
       <c r="G30" s="3">
         <f>IF(C30*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C30*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.36755101653626432</v>
+        <v>0.31981455971512818</v>
       </c>
       <c r="H30" s="3">
         <f>IF(D30*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D30*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.15531728952486967</v>
+        <v>0.1323663538771066</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" si="2"/>
@@ -15045,15 +15045,15 @@
       </c>
       <c r="F31" s="3">
         <f>IF(B31*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B31*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.37513049913771845</v>
+        <v>0.32667802677005708</v>
       </c>
       <c r="G31" s="3">
         <f>IF(C31*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C31*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H31" s="3">
         <f>IF(D31*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D31*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10283058410421708</v>
+        <v>8.7234734950844883E-2</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="2"/>
@@ -15083,15 +15083,15 @@
       </c>
       <c r="F32" s="3">
         <f>IF(B32*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B32*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.5090176207178535</v>
+        <v>0.45029218745214572</v>
       </c>
       <c r="G32" s="3">
         <f>IF(C32*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C32*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="H32" s="3">
         <f>IF(D32*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D32*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" si="2"/>
@@ -15121,15 +15121,15 @@
       </c>
       <c r="F33" s="3">
         <f>IF(B33*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B33*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.585275673072428</v>
+        <v>0.52305500629686519</v>
       </c>
       <c r="G33" s="3">
         <f>IF(C33*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C33*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="H33" s="3">
         <f>IF(D33*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D33*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>5.8502557589133808E-2</v>
+        <v>4.9444934699428233E-2</v>
       </c>
       <c r="J33" s="3">
         <f t="shared" si="2"/>
@@ -15159,15 +15159,15 @@
       </c>
       <c r="F34" s="3">
         <f>IF(B34*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B34*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.40455089961354063</v>
+        <v>0.35344628439351555</v>
       </c>
       <c r="G34" s="3">
         <f>IF(C34*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C34*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H34" s="3">
         <f>IF(D34*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D34*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="J34" s="3">
         <f t="shared" si="2"/>
@@ -15197,15 +15197,15 @@
       </c>
       <c r="F35" s="3">
         <f>IF(B35*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B35*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.59024586972470483</v>
+        <v>0.52786765893159926</v>
       </c>
       <c r="G35" s="3">
         <f>IF(C35*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C35*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.1450715375735252</v>
+        <v>0.12352218246629398</v>
       </c>
       <c r="H35" s="3">
         <f>IF(D35*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D35*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.3825052317163253E-2</v>
+        <v>2.0079344430044999E-2</v>
       </c>
       <c r="J35" s="3">
         <f t="shared" si="2"/>
@@ -15235,15 +15235,15 @@
       </c>
       <c r="F36" s="3">
         <f>IF(B36*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B36*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.38261914665522456</v>
+        <v>0.3334722374469099</v>
       </c>
       <c r="G36" s="3">
         <f>IF(C36*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C36*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H36" s="3">
         <f>IF(D36*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D36*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" si="2"/>
@@ -15273,15 +15273,15 @@
       </c>
       <c r="F37" s="3">
         <f>IF(B37*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B37*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.40455089961354063</v>
+        <v>0.35344628439351555</v>
       </c>
       <c r="G37" s="3">
         <f>IF(C37*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C37*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.24217650602576057</v>
+        <v>0.20805414503107234</v>
       </c>
       <c r="H37" s="3">
         <f>IF(D37*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D37*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="J37" s="3">
         <f t="shared" si="2"/>
@@ -15311,11 +15311,11 @@
       </c>
       <c r="F38" s="3">
         <f>IF(B38*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B38*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12420569237529278</v>
+        <v>0.10556246309154804</v>
       </c>
       <c r="G38" s="3">
         <f>IF(C38*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C38*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>3.5523863170515813E-2</v>
+        <v>2.996731429475108E-2</v>
       </c>
       <c r="H38" s="3" t="str">
         <f>IF(D38*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D38*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -15349,15 +15349,15 @@
       </c>
       <c r="F39" s="3">
         <f>IF(B39*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B39*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.585275673072428</v>
+        <v>0.52305500629686519</v>
       </c>
       <c r="G39" s="3">
         <f>IF(C39*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C39*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.32010393855903041</v>
+        <v>0.27713933178470684</v>
       </c>
       <c r="H39" s="3">
         <f>IF(D39*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D39*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.17544189929334297</v>
+        <v>0.14978786869670402</v>
       </c>
       <c r="J39" s="3">
         <f t="shared" si="2"/>
@@ -15387,15 +15387,15 @@
       </c>
       <c r="F40" s="3">
         <f>IF(B40*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B40*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.56478465918500087</v>
+        <v>0.50330879472078838</v>
       </c>
       <c r="G40" s="3">
         <f>IF(C40*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C40*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.34425647321583208</v>
+        <v>0.2988015246204283</v>
       </c>
       <c r="H40" s="3">
         <f>IF(D40*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D40*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.16544025291826803</v>
+        <v>0.14112128244984734</v>
       </c>
       <c r="J40" s="3">
         <f t="shared" si="2"/>
@@ -15425,15 +15425,15 @@
       </c>
       <c r="F41" s="3">
         <f>IF(B41*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B41*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.49703443993558749</v>
+        <v>0.43902824231404158</v>
       </c>
       <c r="G41" s="3">
         <f>IF(C41*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C41*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.30351002855087539</v>
+        <v>0.26232734853940509</v>
       </c>
       <c r="H41" s="3">
         <f>IF(D41*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D41*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.13470150767527056</v>
+        <v>0.11458785852590458</v>
       </c>
       <c r="J41" s="3">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Update forecast for 7 April 2022
</commit_message>
<xml_diff>
--- a/Forecast/TCs_within_50_miles_1880-2020.xlsx
+++ b/Forecast/TCs_within_50_miles_1880-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmbell/Development/csu-tropical/Forecast/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Phils_Work_Files\Landfalling_Hurricanes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CE2424-AA7A-DF48-8960-AC439E6E4DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2957EF95-75F2-4D66-8F62-3E595B01A2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2740" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="County" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,21 @@
     <sheet name="Caribbean-Central America" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="233">
   <si>
     <t>State</t>
   </si>
@@ -719,6 +729,9 @@
   </si>
   <si>
     <t>NTC Adjustment</t>
+  </si>
+  <si>
+    <t>2022 Probability</t>
   </si>
 </sst>
 </file>
@@ -1045,25 +1058,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" style="3" customWidth="1"/>
-    <col min="14" max="22" width="7.6640625" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="12.6640625" style="1"/>
+    <col min="10" max="10" width="7.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.25" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.125" style="3" customWidth="1"/>
+    <col min="14" max="22" width="7.625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="12.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1071,19 +1084,19 @@
         <v>231</v>
       </c>
       <c r="B1" s="14">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H2" s="22">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="15"/>
       <c r="C3" s="5" t="s">
         <v>228</v>
@@ -1114,7 +1127,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
@@ -1169,15 +1182,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="19">
         <f>(1-(1/(2.71828^((C5*($B$1/100))/141))))</f>
-        <v>0.32667802677005708</v>
+        <v>0.37513049913771845</v>
       </c>
       <c r="H5" s="19">
         <f t="shared" ref="H5" si="0">(1-(1/(2.71828^((D5*($B$1/100))/141))))</f>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="I5" s="19">
         <f>IF(E5*($B$1/100)&gt;0, (1-(1/(2.71828^(E5*($B$1/100)/141)))), "&lt;1%")</f>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K5" s="2">
         <f>(1-(1/(2.71828^(C5/141))))</f>
@@ -1192,7 +1205,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -1211,15 +1224,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="19">
         <f t="shared" ref="G6:G69" si="1">(1-(1/(2.71828^((C6*($B$1/100))/141))))</f>
-        <v>0.2988015246204283</v>
+        <v>0.34425647321583208</v>
       </c>
       <c r="H6" s="19">
         <f t="shared" ref="H6:H69" si="2">(1-(1/(2.71828^((D6*($B$1/100))/141))))</f>
-        <v>0.17526644285268</v>
+        <v>0.2047333884389867</v>
       </c>
       <c r="I6" s="19">
         <f t="shared" ref="I6:I69" si="3">IF(E6*($B$1/100)&gt;0, (1-(1/(2.71828^(E6*($B$1/100)/141)))), "&lt;1%")</f>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ref="K6:K69" si="4">(1-(1/(2.71828^(C6/141))))</f>
@@ -1234,7 +1247,7 @@
         <v>5.5157989846188027E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -1253,15 +1266,15 @@
       <c r="F7" s="6"/>
       <c r="G7" s="19">
         <f t="shared" si="1"/>
-        <v>0.32667802677005708</v>
+        <v>0.37513049913771845</v>
       </c>
       <c r="H7" s="19">
         <f t="shared" si="2"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="I7" s="19">
         <f t="shared" si="3"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ref="K7" si="7">(1-(1/(2.71828^(C7/141))))</f>
@@ -1276,7 +1289,7 @@
         <v>6.846539335832047E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
@@ -1294,15 +1307,15 @@
       </c>
       <c r="G8" s="19">
         <f t="shared" si="1"/>
-        <v>0.30587702543196937</v>
+        <v>0.3521151255059447</v>
       </c>
       <c r="H8" s="19">
         <f t="shared" si="2"/>
-        <v>0.17526644285268</v>
+        <v>0.2047333884389867</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="4"/>
@@ -1317,7 +1330,7 @@
         <v>5.5157989846188027E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -1335,15 +1348,15 @@
       </c>
       <c r="G9" s="19">
         <f t="shared" si="1"/>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="H9" s="19">
         <f t="shared" si="2"/>
-        <v>0.15836700404317228</v>
+        <v>0.18532368255428877</v>
       </c>
       <c r="I9" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="4"/>
@@ -1358,7 +1371,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
@@ -1376,15 +1389,15 @@
       </c>
       <c r="G10" s="19">
         <f t="shared" si="1"/>
-        <v>0.32667802677005708</v>
+        <v>0.37513049913771845</v>
       </c>
       <c r="H10" s="19">
         <f t="shared" si="2"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="I10" s="19">
         <f t="shared" si="3"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="4"/>
@@ -1399,7 +1412,7 @@
         <v>6.1835286174562576E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>5</v>
       </c>
@@ -1417,15 +1430,15 @@
       </c>
       <c r="G11" s="19">
         <f t="shared" si="1"/>
-        <v>0.26232734853940509</v>
+        <v>0.30351002855087539</v>
       </c>
       <c r="H11" s="19">
         <f t="shared" si="2"/>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="I11" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="4"/>
@@ -1440,7 +1453,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>5</v>
       </c>
@@ -1458,15 +1471,15 @@
       </c>
       <c r="G12" s="19">
         <f t="shared" si="1"/>
-        <v>0.34019789058285854</v>
+        <v>0.39001804768716197</v>
       </c>
       <c r="H12" s="19">
         <f t="shared" si="2"/>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="I12" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" si="4"/>
@@ -1481,7 +1494,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -1499,15 +1512,15 @@
       </c>
       <c r="G13" s="19">
         <f t="shared" si="1"/>
-        <v>0.42169808713392831</v>
+        <v>0.47850906740128607</v>
       </c>
       <c r="H13" s="19">
         <f t="shared" si="2"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="I13" s="19">
         <f t="shared" si="3"/>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="4"/>
@@ -1522,7 +1535,7 @@
         <v>7.5048644888033755E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
@@ -1540,15 +1553,15 @@
       </c>
       <c r="G14" s="19">
         <f t="shared" si="1"/>
-        <v>0.40383254978091254</v>
+        <v>0.45930136300416158</v>
       </c>
       <c r="H14" s="19">
         <f t="shared" si="2"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="I14" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="4"/>
@@ -1563,7 +1576,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>5</v>
       </c>
@@ -1581,15 +1594,15 @@
       </c>
       <c r="G15" s="19">
         <f t="shared" si="1"/>
-        <v>0.44468877391261652</v>
+        <v>0.50306214938143157</v>
       </c>
       <c r="H15" s="19">
         <f t="shared" si="2"/>
-        <v>0.25480792671460639</v>
+        <v>0.29506181078156346</v>
       </c>
       <c r="I15" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="4"/>
@@ -1604,7 +1617,7 @@
         <v>5.5157989846188027E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
@@ -1622,15 +1635,15 @@
       </c>
       <c r="G16" s="19">
         <f t="shared" si="1"/>
-        <v>0.40383254978091254</v>
+        <v>0.45930136300416158</v>
       </c>
       <c r="H16" s="19">
         <f t="shared" si="2"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="I16" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="4"/>
@@ -1645,7 +1658,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
@@ -1663,15 +1676,15 @@
       </c>
       <c r="G17" s="19">
         <f t="shared" si="1"/>
-        <v>0.39161661015060845</v>
+        <v>0.4461047804194278</v>
       </c>
       <c r="H17" s="19">
         <f t="shared" si="2"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="I17" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="4"/>
@@ -1686,7 +1699,7 @@
         <v>4.1660483908474766E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -1704,15 +1717,15 @@
       </c>
       <c r="G18" s="19">
         <f t="shared" si="1"/>
-        <v>0.39161661015060845</v>
+        <v>0.4461047804194278</v>
       </c>
       <c r="H18" s="19">
         <f t="shared" si="2"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="I18" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="4"/>
@@ -1727,7 +1740,7 @@
         <v>4.1660483908474766E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
@@ -1745,15 +1758,15 @@
       </c>
       <c r="G19" s="19">
         <f t="shared" si="1"/>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="H19" s="19">
         <f t="shared" si="2"/>
-        <v>0.1323663538771066</v>
+        <v>0.15531728952486967</v>
       </c>
       <c r="I19" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="4"/>
@@ -1768,7 +1781,7 @@
         <v>4.1660483908474766E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>19</v>
       </c>
@@ -1786,15 +1799,15 @@
       </c>
       <c r="G20" s="19">
         <f t="shared" si="1"/>
-        <v>0.41580320135184334</v>
+        <v>0.47218353631840626</v>
       </c>
       <c r="H20" s="19">
         <f t="shared" si="2"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="I20" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="4"/>
@@ -1809,7 +1822,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>19</v>
       </c>
@@ -1827,15 +1840,15 @@
       </c>
       <c r="G21" s="19">
         <f t="shared" si="1"/>
-        <v>0.4098482264059311</v>
+        <v>0.46578127841061079</v>
       </c>
       <c r="H21" s="19">
         <f t="shared" si="2"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="I21" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="4"/>
@@ -1850,7 +1863,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
@@ -1868,15 +1881,15 @@
       </c>
       <c r="G22" s="19">
         <f t="shared" si="1"/>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="H22" s="19">
         <f t="shared" si="2"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="I22" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" si="4"/>
@@ -1891,7 +1904,7 @@
         <v>4.8433168509038227E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>19</v>
       </c>
@@ -1909,15 +1922,15 @@
       </c>
       <c r="G23" s="19">
         <f t="shared" si="1"/>
-        <v>0.46132995995618065</v>
+        <v>0.52071530159105595</v>
       </c>
       <c r="H23" s="19">
         <f t="shared" si="2"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="I23" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K23" s="2">
         <f t="shared" si="4"/>
@@ -1932,7 +1945,7 @@
         <v>4.1660483908474766E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>19</v>
       </c>
@@ -1950,15 +1963,15 @@
       </c>
       <c r="G24" s="19">
         <f t="shared" si="1"/>
-        <v>0.55121221170521451</v>
+        <v>0.61421753432852066</v>
       </c>
       <c r="H24" s="19">
         <f t="shared" si="2"/>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="I24" s="19">
         <f t="shared" si="3"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="4"/>
@@ -1973,7 +1986,7 @@
         <v>6.1835286174562576E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>19</v>
       </c>
@@ -1991,15 +2004,15 @@
       </c>
       <c r="G25" s="19">
         <f t="shared" si="1"/>
-        <v>0.51328202850696369</v>
+        <v>0.57515368744915019</v>
       </c>
       <c r="H25" s="19">
         <f t="shared" si="2"/>
-        <v>0.28443341673236711</v>
+        <v>0.32825204299627064</v>
       </c>
       <c r="I25" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K25" s="2">
         <f t="shared" si="4"/>
@@ -2032,15 +2045,15 @@
       </c>
       <c r="G26" s="19">
         <f t="shared" si="1"/>
-        <v>0.4931312015355781</v>
+        <v>0.5541625588240332</v>
       </c>
       <c r="H26" s="19">
         <f t="shared" si="2"/>
-        <v>0.26232734853940509</v>
+        <v>0.30351002855087539</v>
       </c>
       <c r="I26" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="4"/>
@@ -2073,15 +2086,15 @@
       </c>
       <c r="G27" s="19">
         <f t="shared" si="1"/>
-        <v>0.55574074174597166</v>
+        <v>0.61884088192327691</v>
       </c>
       <c r="H27" s="19">
         <f t="shared" si="2"/>
-        <v>0.2988015246204283</v>
+        <v>0.34425647321583208</v>
       </c>
       <c r="I27" s="19">
         <f t="shared" si="3"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="4"/>
@@ -2114,15 +2127,15 @@
       </c>
       <c r="G28" s="19">
         <f t="shared" si="1"/>
-        <v>0.52786765893159926</v>
+        <v>0.59024586972470483</v>
       </c>
       <c r="H28" s="19">
         <f t="shared" si="2"/>
-        <v>0.28443341673236711</v>
+        <v>0.32825204299627064</v>
       </c>
       <c r="I28" s="19">
         <f t="shared" si="3"/>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" si="4"/>
@@ -2155,15 +2168,15 @@
       </c>
       <c r="G29" s="19">
         <f t="shared" si="1"/>
-        <v>0.42169808713392831</v>
+        <v>0.47850906740128607</v>
       </c>
       <c r="H29" s="19">
         <f t="shared" si="2"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="I29" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K29" s="2">
         <f t="shared" si="4"/>
@@ -2196,15 +2209,15 @@
       </c>
       <c r="G30" s="19">
         <f t="shared" si="1"/>
-        <v>0.44468877391261652</v>
+        <v>0.50306214938143157</v>
       </c>
       <c r="H30" s="19">
         <f t="shared" si="2"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="I30" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" si="4"/>
@@ -2237,15 +2250,15 @@
       </c>
       <c r="G31" s="19">
         <f t="shared" si="1"/>
-        <v>0.42169808713392831</v>
+        <v>0.47850906740128607</v>
       </c>
       <c r="H31" s="19">
         <f t="shared" si="2"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I31" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" si="4"/>
@@ -2278,15 +2291,15 @@
       </c>
       <c r="G32" s="19">
         <f t="shared" si="1"/>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="H32" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I32" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="4"/>
@@ -2319,15 +2332,15 @@
       </c>
       <c r="G33" s="19">
         <f t="shared" si="1"/>
-        <v>0.42753349008682928</v>
+        <v>0.48475879117948029</v>
       </c>
       <c r="H33" s="19">
         <f t="shared" si="2"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="I33" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="4"/>
@@ -2360,15 +2373,15 @@
       </c>
       <c r="G34" s="19">
         <f t="shared" si="1"/>
-        <v>0.4931312015355781</v>
+        <v>0.5541625588240332</v>
       </c>
       <c r="H34" s="19">
         <f t="shared" si="2"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="I34" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" si="4"/>
@@ -2401,15 +2414,15 @@
       </c>
       <c r="G35" s="19">
         <f t="shared" si="1"/>
-        <v>0.53263174909961608</v>
+        <v>0.59515650185867774</v>
       </c>
       <c r="H35" s="19">
         <f t="shared" si="2"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="I35" s="19">
         <f t="shared" si="3"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="4"/>
@@ -2442,15 +2455,15 @@
       </c>
       <c r="G36" s="19">
         <f t="shared" si="1"/>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="H36" s="19">
         <f t="shared" si="2"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="I36" s="19">
         <f t="shared" si="3"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" si="4"/>
@@ -2483,15 +2496,15 @@
       </c>
       <c r="G37" s="19">
         <f t="shared" si="1"/>
-        <v>0.46132995995618065</v>
+        <v>0.52071530159105595</v>
       </c>
       <c r="H37" s="19">
         <f t="shared" si="2"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="I37" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K37" s="2">
         <f t="shared" si="4"/>
@@ -2524,15 +2537,15 @@
       </c>
       <c r="G38" s="19">
         <f t="shared" si="1"/>
-        <v>0.46676545424104743</v>
+        <v>0.52645921157860687</v>
       </c>
       <c r="H38" s="19">
         <f t="shared" si="2"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="I38" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K38" s="2">
         <f t="shared" si="4"/>
@@ -2565,15 +2578,15 @@
       </c>
       <c r="G39" s="19">
         <f t="shared" si="1"/>
-        <v>0.45583905928709567</v>
+        <v>0.51490171967079768</v>
       </c>
       <c r="H39" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I39" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K39" s="2">
         <f t="shared" si="4"/>
@@ -2606,15 +2619,15 @@
       </c>
       <c r="G40" s="19">
         <f t="shared" si="1"/>
-        <v>0.44468877391261652</v>
+        <v>0.50306214938143157</v>
       </c>
       <c r="H40" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I40" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K40" s="2">
         <f t="shared" si="4"/>
@@ -2647,15 +2660,15 @@
       </c>
       <c r="G41" s="19">
         <f t="shared" si="1"/>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="H41" s="19">
         <f t="shared" si="2"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="I41" s="19">
         <f t="shared" si="3"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K41" s="2">
         <f t="shared" si="4"/>
@@ -2688,15 +2701,15 @@
       </c>
       <c r="G42" s="19">
         <f t="shared" si="1"/>
-        <v>0.45583905928709567</v>
+        <v>0.51490171967079768</v>
       </c>
       <c r="H42" s="19">
         <f t="shared" si="2"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="I42" s="19">
         <f t="shared" si="3"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K42" s="2">
         <f t="shared" si="4"/>
@@ -2729,15 +2742,15 @@
       </c>
       <c r="G43" s="19">
         <f t="shared" si="1"/>
-        <v>0.42169808713392831</v>
+        <v>0.47850906740128607</v>
       </c>
       <c r="H43" s="19">
         <f t="shared" si="2"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="I43" s="19">
         <f t="shared" si="3"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K43" s="2">
         <f t="shared" si="4"/>
@@ -2770,15 +2783,15 @@
       </c>
       <c r="G44" s="19">
         <f t="shared" si="1"/>
-        <v>0.43331001042692008</v>
+        <v>0.49093361615337672</v>
       </c>
       <c r="H44" s="19">
         <f t="shared" si="2"/>
-        <v>0.1323663538771066</v>
+        <v>0.15531728952486967</v>
       </c>
       <c r="I44" s="19">
         <f t="shared" si="3"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K44" s="2">
         <f t="shared" si="4"/>
@@ -2811,15 +2824,15 @@
       </c>
       <c r="G45" s="19">
         <f t="shared" si="1"/>
-        <v>0.46676545424104743</v>
+        <v>0.52645921157860687</v>
       </c>
       <c r="H45" s="19">
         <f t="shared" si="2"/>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="I45" s="19">
         <f t="shared" si="3"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" si="4"/>
@@ -2852,15 +2865,15 @@
       </c>
       <c r="G46" s="19">
         <f t="shared" si="1"/>
-        <v>0.46132995995618065</v>
+        <v>0.52071530159105595</v>
       </c>
       <c r="H46" s="19">
         <f t="shared" si="2"/>
-        <v>0.17526644285268</v>
+        <v>0.2047333884389867</v>
       </c>
       <c r="I46" s="19">
         <f t="shared" si="3"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K46" s="2">
         <f t="shared" si="4"/>
@@ -2893,15 +2906,15 @@
       </c>
       <c r="G47" s="19">
         <f t="shared" si="1"/>
-        <v>0.46676545424104743</v>
+        <v>0.52645921157860687</v>
       </c>
       <c r="H47" s="19">
         <f t="shared" si="2"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I47" s="19">
         <f t="shared" si="3"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K47" s="2">
         <f t="shared" si="4"/>
@@ -2934,15 +2947,15 @@
       </c>
       <c r="G48" s="19">
         <f t="shared" si="1"/>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="H48" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I48" s="19">
         <f t="shared" si="3"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K48" s="2">
         <f t="shared" si="4"/>
@@ -2975,15 +2988,15 @@
       </c>
       <c r="G49" s="19">
         <f t="shared" si="1"/>
-        <v>0.44468877391261652</v>
+        <v>0.50306214938143157</v>
       </c>
       <c r="H49" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I49" s="19">
         <f t="shared" si="3"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K49" s="2">
         <f t="shared" si="4"/>
@@ -3016,15 +3029,15 @@
       </c>
       <c r="G50" s="19">
         <f t="shared" si="1"/>
-        <v>0.47214610122436662</v>
+        <v>0.53213428460546475</v>
       </c>
       <c r="H50" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I50" s="19">
         <f t="shared" si="3"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K50" s="2">
         <f t="shared" si="4"/>
@@ -3057,15 +3070,15 @@
       </c>
       <c r="G51" s="19">
         <f t="shared" si="1"/>
-        <v>0.47747245434733998</v>
+        <v>0.53774134563705722</v>
       </c>
       <c r="H51" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I51" s="19">
         <f t="shared" si="3"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="K51" s="2">
         <f t="shared" si="4"/>
@@ -3098,15 +3111,15 @@
       </c>
       <c r="G52" s="19">
         <f t="shared" si="1"/>
-        <v>0.47214610122436662</v>
+        <v>0.53213428460546475</v>
       </c>
       <c r="H52" s="19">
         <f t="shared" si="2"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="I52" s="19">
         <f t="shared" si="3"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="K52" s="2">
         <f t="shared" si="4"/>
@@ -3139,15 +3152,15 @@
       </c>
       <c r="G53" s="19">
         <f t="shared" si="1"/>
-        <v>0.48274506146662466</v>
+        <v>0.54328120975214667</v>
       </c>
       <c r="H53" s="19">
         <f t="shared" si="2"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="I53" s="19">
         <f t="shared" si="3"/>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="K53" s="2">
         <f t="shared" si="4"/>
@@ -3180,15 +3193,15 @@
       </c>
       <c r="G54" s="19">
         <f t="shared" si="1"/>
-        <v>0.47214610122436662</v>
+        <v>0.53213428460546475</v>
       </c>
       <c r="H54" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I54" s="19">
         <f t="shared" si="3"/>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="K54" s="2">
         <f t="shared" si="4"/>
@@ -3221,15 +3234,15 @@
       </c>
       <c r="G55" s="19">
         <f t="shared" si="1"/>
-        <v>0.4931312015355781</v>
+        <v>0.5541625588240332</v>
       </c>
       <c r="H55" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I55" s="19">
         <f t="shared" si="3"/>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="K55" s="2">
         <f t="shared" si="4"/>
@@ -3262,15 +3275,15 @@
       </c>
       <c r="G56" s="19">
         <f t="shared" si="1"/>
-        <v>0.51328202850696369</v>
+        <v>0.57515368744915019</v>
       </c>
       <c r="H56" s="19">
         <f t="shared" si="2"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="I56" s="19">
         <f t="shared" si="3"/>
-        <v>0.15836700404317228</v>
+        <v>0.18532368255428877</v>
       </c>
       <c r="K56" s="2">
         <f t="shared" si="4"/>
@@ -3303,15 +3316,15 @@
       </c>
       <c r="G57" s="19">
         <f t="shared" si="1"/>
-        <v>0.54201619718511251</v>
+        <v>0.6048019193821581</v>
       </c>
       <c r="H57" s="19">
         <f t="shared" si="2"/>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="I57" s="19">
         <f t="shared" si="3"/>
-        <v>0.17526644285268</v>
+        <v>0.2047333884389867</v>
       </c>
       <c r="K57" s="2">
         <f t="shared" si="4"/>
@@ -3344,15 +3357,15 @@
       </c>
       <c r="G58" s="19">
         <f t="shared" si="1"/>
-        <v>0.64817072189415192</v>
+        <v>0.71114866537895804</v>
       </c>
       <c r="H58" s="19">
         <f t="shared" si="2"/>
-        <v>0.39775555271787122</v>
+        <v>0.45274284813652177</v>
       </c>
       <c r="I58" s="19">
         <f t="shared" si="3"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="K58" s="2">
         <f t="shared" si="4"/>
@@ -3385,15 +3398,15 @@
       </c>
       <c r="G59" s="19">
         <f t="shared" si="1"/>
-        <v>0.55121221170521451</v>
+        <v>0.61421753432852066</v>
       </c>
       <c r="H59" s="19">
         <f t="shared" si="2"/>
-        <v>0.31288113032139719</v>
+        <v>0.3598795970481059</v>
       </c>
       <c r="I59" s="19">
         <f t="shared" si="3"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="K59" s="2">
         <f t="shared" si="4"/>
@@ -3426,15 +3439,15 @@
       </c>
       <c r="G60" s="19">
         <f t="shared" si="1"/>
-        <v>0.54201619718511251</v>
+        <v>0.6048019193821581</v>
       </c>
       <c r="H60" s="19">
         <f t="shared" si="2"/>
-        <v>0.30587702543196937</v>
+        <v>0.3521151255059447</v>
       </c>
       <c r="I60" s="19">
         <f t="shared" si="3"/>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="K60" s="2">
         <f t="shared" si="4"/>
@@ -3467,15 +3480,15 @@
       </c>
       <c r="G61" s="19">
         <f t="shared" si="1"/>
-        <v>0.54201619718511251</v>
+        <v>0.6048019193821581</v>
       </c>
       <c r="H61" s="19">
         <f t="shared" si="2"/>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="I61" s="19">
         <f t="shared" si="3"/>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="K61" s="2">
         <f t="shared" si="4"/>
@@ -3508,15 +3521,15 @@
       </c>
       <c r="G62" s="19">
         <f t="shared" si="1"/>
-        <v>0.4931312015355781</v>
+        <v>0.5541625588240332</v>
       </c>
       <c r="H62" s="19">
         <f t="shared" si="2"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="I62" s="19">
         <f t="shared" si="3"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="K62" s="2">
         <f t="shared" si="4"/>
@@ -3549,15 +3562,15 @@
       </c>
       <c r="G63" s="19">
         <f t="shared" si="1"/>
-        <v>0.47214610122436662</v>
+        <v>0.53213428460546475</v>
       </c>
       <c r="H63" s="19">
         <f t="shared" si="2"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="I63" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K63" s="2">
         <f t="shared" si="4"/>
@@ -3590,15 +3603,15 @@
       </c>
       <c r="G64" s="19">
         <f t="shared" si="1"/>
-        <v>0.48274506146662466</v>
+        <v>0.54328120975214667</v>
       </c>
       <c r="H64" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I64" s="19">
         <f t="shared" si="3"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="K64" s="2">
         <f t="shared" si="4"/>
@@ -3631,15 +3644,15 @@
       </c>
       <c r="G65" s="19">
         <f t="shared" si="1"/>
-        <v>0.54663752036573587</v>
+        <v>0.60953810689212307</v>
       </c>
       <c r="H65" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I65" s="19">
         <f t="shared" si="3"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="K65" s="2">
         <f t="shared" si="4"/>
@@ -3672,15 +3685,15 @@
       </c>
       <c r="G66" s="19">
         <f t="shared" si="1"/>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="H66" s="19">
         <f t="shared" si="2"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I66" s="19">
         <f t="shared" si="3"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="K66" s="2">
         <f t="shared" si="4"/>
@@ -3713,15 +3726,15 @@
       </c>
       <c r="G67" s="19">
         <f t="shared" si="1"/>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="H67" s="19">
         <f t="shared" si="2"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I67" s="19">
         <f t="shared" si="3"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="K67" s="2">
         <f t="shared" si="4"/>
@@ -3754,15 +3767,15 @@
       </c>
       <c r="G68" s="19">
         <f t="shared" si="1"/>
-        <v>0.4982458027801665</v>
+        <v>0.55950562556431493</v>
       </c>
       <c r="H68" s="19">
         <f t="shared" si="2"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="I68" s="19">
         <f t="shared" si="3"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K68" s="2">
         <f t="shared" si="4"/>
@@ -3795,15 +3808,15 @@
       </c>
       <c r="G69" s="19">
         <f t="shared" si="1"/>
-        <v>0.4931312015355781</v>
+        <v>0.5541625588240332</v>
       </c>
       <c r="H69" s="19">
         <f t="shared" si="2"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I69" s="19">
         <f t="shared" si="3"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K69" s="2">
         <f t="shared" si="4"/>
@@ -3836,15 +3849,15 @@
       </c>
       <c r="G70" s="19">
         <f t="shared" ref="G70:G133" si="10">(1-(1/(2.71828^((C70*($B$1/100))/141))))</f>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="H70" s="19">
         <f t="shared" ref="H70:H133" si="11">(1-(1/(2.71828^((D70*($B$1/100))/141))))</f>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="I70" s="19">
         <f t="shared" ref="I70:I133" si="12">IF(E70*($B$1/100)&gt;0, (1-(1/(2.71828^(E70*($B$1/100)/141)))), "&lt;1%")</f>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K70" s="2">
         <f t="shared" ref="K70:K132" si="13">(1-(1/(2.71828^(C70/141))))</f>
@@ -3877,15 +3890,15 @@
       </c>
       <c r="G71" s="19">
         <f t="shared" si="10"/>
-        <v>0.51819329617682908</v>
+        <v>0.58024518940182213</v>
       </c>
       <c r="H71" s="19">
         <f t="shared" si="11"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="I71" s="19">
         <f t="shared" si="12"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K71" s="2">
         <f t="shared" si="13"/>
@@ -3918,15 +3931,15 @@
       </c>
       <c r="G72" s="19">
         <f t="shared" si="10"/>
-        <v>0.47747245434733998</v>
+        <v>0.53774134563705722</v>
       </c>
       <c r="H72" s="19">
         <f t="shared" si="11"/>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="I72" s="19">
         <f t="shared" si="12"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K72" s="2">
         <f t="shared" si="13"/>
@@ -3959,15 +3972,15 @@
       </c>
       <c r="G73" s="19">
         <f t="shared" si="10"/>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="H73" s="19">
         <f t="shared" si="11"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="I73" s="19">
         <f t="shared" si="12"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K73" s="2">
         <f t="shared" si="13"/>
@@ -4000,15 +4013,15 @@
       </c>
       <c r="G74" s="19">
         <f t="shared" si="10"/>
-        <v>0.51819329617682908</v>
+        <v>0.58024518940182213</v>
       </c>
       <c r="H74" s="19">
         <f t="shared" si="11"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I74" s="19">
         <f t="shared" si="12"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K74" s="2">
         <f t="shared" si="13"/>
@@ -4041,15 +4054,15 @@
       </c>
       <c r="G75" s="19">
         <f t="shared" si="10"/>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="H75" s="19">
         <f t="shared" si="11"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="I75" s="19">
         <f t="shared" si="12"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="K75" s="2">
         <f t="shared" si="13"/>
@@ -4082,15 +4095,15 @@
       </c>
       <c r="G76" s="19">
         <f t="shared" si="10"/>
-        <v>0.51819329617682908</v>
+        <v>0.58024518940182213</v>
       </c>
       <c r="H76" s="19">
         <f t="shared" si="11"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I76" s="19">
         <f t="shared" si="12"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K76" s="2">
         <f t="shared" si="13"/>
@@ -4123,15 +4136,15 @@
       </c>
       <c r="G77" s="19">
         <f t="shared" si="10"/>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="H77" s="19">
         <f t="shared" si="11"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="I77" s="19">
         <f t="shared" si="12"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="K77" s="2">
         <f t="shared" si="13"/>
@@ -4164,15 +4177,15 @@
       </c>
       <c r="G78" s="19">
         <f t="shared" si="10"/>
-        <v>0.4931312015355781</v>
+        <v>0.5541625588240332</v>
       </c>
       <c r="H78" s="19">
         <f t="shared" si="11"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I78" s="19">
         <f t="shared" si="12"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K78" s="2">
         <f t="shared" si="13"/>
@@ -4205,15 +4218,15 @@
       </c>
       <c r="G79" s="19">
         <f t="shared" si="10"/>
-        <v>0.51328202850696369</v>
+        <v>0.57515368744915019</v>
       </c>
       <c r="H79" s="19">
         <f t="shared" si="11"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I79" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K79" s="2">
         <f t="shared" si="13"/>
@@ -4246,15 +4259,15 @@
       </c>
       <c r="G80" s="19">
         <f t="shared" si="10"/>
-        <v>0.55574074174597166</v>
+        <v>0.61884088192327691</v>
       </c>
       <c r="H80" s="19">
         <f t="shared" si="11"/>
-        <v>0.28443341673236711</v>
+        <v>0.32825204299627064</v>
       </c>
       <c r="I80" s="19">
         <f t="shared" si="12"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="K80" s="2">
         <f t="shared" si="13"/>
@@ -4287,15 +4300,15 @@
       </c>
       <c r="G81" s="19">
         <f t="shared" si="10"/>
-        <v>0.47747245434733998</v>
+        <v>0.53774134563705722</v>
       </c>
       <c r="H81" s="19">
         <f t="shared" si="11"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="I81" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K81" s="2">
         <f t="shared" si="13"/>
@@ -4328,15 +4341,15 @@
       </c>
       <c r="G82" s="19">
         <f t="shared" si="10"/>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="H82" s="19">
         <f t="shared" si="11"/>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="I82" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K82" s="2">
         <f t="shared" si="13"/>
@@ -4369,15 +4382,15 @@
       </c>
       <c r="G83" s="19">
         <f t="shared" si="10"/>
-        <v>0.52786765893159926</v>
+        <v>0.59024586972470483</v>
       </c>
       <c r="H83" s="19">
         <f t="shared" si="11"/>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="I83" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K83" s="2">
         <f t="shared" si="13"/>
@@ -4410,15 +4423,15 @@
       </c>
       <c r="G84" s="19">
         <f t="shared" si="10"/>
-        <v>0.51328202850696369</v>
+        <v>0.57515368744915019</v>
       </c>
       <c r="H84" s="19">
         <f t="shared" si="11"/>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="I84" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K84" s="2">
         <f t="shared" si="13"/>
@@ -4451,15 +4464,15 @@
       </c>
       <c r="G85" s="19">
         <f t="shared" si="10"/>
-        <v>0.53734776682447505</v>
+        <v>0.60000828331568745</v>
       </c>
       <c r="H85" s="19">
         <f t="shared" si="11"/>
-        <v>0.2988015246204283</v>
+        <v>0.34425647321583208</v>
       </c>
       <c r="I85" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K85" s="2">
         <f t="shared" si="13"/>
@@ -4492,15 +4505,15 @@
       </c>
       <c r="G86" s="19">
         <f t="shared" si="10"/>
-        <v>0.52786765893159926</v>
+        <v>0.59024586972470483</v>
       </c>
       <c r="H86" s="19">
         <f t="shared" si="11"/>
-        <v>0.2988015246204283</v>
+        <v>0.34425647321583208</v>
       </c>
       <c r="I86" s="19">
         <f t="shared" si="12"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K86" s="2">
         <f t="shared" si="13"/>
@@ -4533,15 +4546,15 @@
       </c>
       <c r="G87" s="19">
         <f t="shared" si="10"/>
-        <v>0.60664745877960757</v>
+        <v>0.67018358979238801</v>
       </c>
       <c r="H87" s="19">
         <f t="shared" si="11"/>
-        <v>0.37282176279753421</v>
+        <v>0.425703551980676</v>
       </c>
       <c r="I87" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K87" s="2">
         <f t="shared" si="13"/>
@@ -4574,15 +4587,15 @@
       </c>
       <c r="G88" s="19">
         <f t="shared" si="10"/>
-        <v>0.62609674949410399</v>
+        <v>0.68947869332440015</v>
       </c>
       <c r="H88" s="19">
         <f t="shared" si="11"/>
-        <v>0.36642865914170353</v>
+        <v>0.41873750558245582</v>
       </c>
       <c r="I88" s="19">
         <f t="shared" si="12"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="K88" s="2">
         <f t="shared" si="13"/>
@@ -4615,15 +4628,15 @@
       </c>
       <c r="G89" s="19">
         <f t="shared" si="10"/>
-        <v>0.61454571993720519</v>
+        <v>0.67804148302064327</v>
       </c>
       <c r="H89" s="19">
         <f t="shared" si="11"/>
-        <v>0.36642865914170353</v>
+        <v>0.41873750558245582</v>
       </c>
       <c r="I89" s="19">
         <f t="shared" si="12"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="K89" s="2">
         <f t="shared" si="13"/>
@@ -4656,15 +4669,15 @@
       </c>
       <c r="G90" s="19">
         <f t="shared" si="10"/>
-        <v>0.47214610122436662</v>
+        <v>0.53213428460546475</v>
       </c>
       <c r="H90" s="19">
         <f t="shared" si="11"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I90" s="19">
         <f t="shared" si="12"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K90" s="2">
         <f t="shared" si="13"/>
@@ -4697,15 +4710,15 @@
       </c>
       <c r="G91" s="19">
         <f t="shared" si="10"/>
-        <v>0.48796446491068579</v>
+        <v>0.54875468226131585</v>
       </c>
       <c r="H91" s="19">
         <f t="shared" si="11"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="I91" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K91" s="2">
         <f t="shared" si="13"/>
@@ -4738,15 +4751,15 @@
       </c>
       <c r="G92" s="19">
         <f t="shared" si="10"/>
-        <v>0.43902824231404158</v>
+        <v>0.49703443993558749</v>
       </c>
       <c r="H92" s="19">
         <f t="shared" si="11"/>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="I92" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K92" s="2">
         <f t="shared" si="13"/>
@@ -4779,15 +4792,15 @@
       </c>
       <c r="G93" s="19">
         <f t="shared" si="10"/>
-        <v>0.46132995995618065</v>
+        <v>0.52071530159105595</v>
       </c>
       <c r="H93" s="19">
         <f t="shared" si="11"/>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="I93" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K93" s="2">
         <f t="shared" si="13"/>
@@ -4820,15 +4833,15 @@
       </c>
       <c r="G94" s="19">
         <f t="shared" si="10"/>
-        <v>0.39161661015060845</v>
+        <v>0.4461047804194278</v>
       </c>
       <c r="H94" s="19">
         <f t="shared" si="11"/>
-        <v>0.15836700404317228</v>
+        <v>0.18532368255428877</v>
       </c>
       <c r="I94" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K94" s="2">
         <f t="shared" si="13"/>
@@ -4861,15 +4874,15 @@
       </c>
       <c r="G95" s="19">
         <f t="shared" si="10"/>
-        <v>0.53734776682447505</v>
+        <v>0.60000828331568745</v>
       </c>
       <c r="H95" s="19">
         <f t="shared" si="11"/>
-        <v>0.26977089502064311</v>
+        <v>0.31185700002005889</v>
       </c>
       <c r="I95" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K95" s="2">
         <f t="shared" si="13"/>
@@ -4902,11 +4915,11 @@
       </c>
       <c r="G96" s="19">
         <f t="shared" si="10"/>
-        <v>0.34019789058285854</v>
+        <v>0.39001804768716197</v>
       </c>
       <c r="H96" s="19">
         <f t="shared" si="11"/>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="I96" s="19" t="str">
         <f t="shared" si="12"/>
@@ -4943,11 +4956,11 @@
       </c>
       <c r="G97" s="19">
         <f t="shared" si="10"/>
-        <v>0.37282176279753421</v>
+        <v>0.425703551980676</v>
       </c>
       <c r="H97" s="19">
         <f t="shared" si="11"/>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="I97" s="19" t="str">
         <f t="shared" si="12"/>
@@ -4984,15 +4997,15 @@
       </c>
       <c r="G98" s="19">
         <f t="shared" si="10"/>
-        <v>0.52305500629686519</v>
+        <v>0.585275673072428</v>
       </c>
       <c r="H98" s="19">
         <f t="shared" si="11"/>
-        <v>0.26977089502064311</v>
+        <v>0.31185700002005889</v>
       </c>
       <c r="I98" s="19">
         <f t="shared" si="12"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K98" s="2">
         <f t="shared" si="13"/>
@@ -5025,15 +5038,15 @@
       </c>
       <c r="G99" s="19">
         <f t="shared" si="10"/>
-        <v>0.42753349008682928</v>
+        <v>0.48475879117948029</v>
       </c>
       <c r="H99" s="19">
         <f t="shared" si="11"/>
-        <v>0.17526644285268</v>
+        <v>0.2047333884389867</v>
       </c>
       <c r="I99" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K99" s="2">
         <f t="shared" si="13"/>
@@ -5066,15 +5079,15 @@
       </c>
       <c r="G100" s="19">
         <f t="shared" si="10"/>
-        <v>0.4098482264059311</v>
+        <v>0.46578127841061079</v>
       </c>
       <c r="H100" s="19">
         <f t="shared" si="11"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="I100" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K100" s="2">
         <f t="shared" si="13"/>
@@ -5107,15 +5120,15 @@
       </c>
       <c r="G101" s="19">
         <f t="shared" si="10"/>
-        <v>0.47747245434733998</v>
+        <v>0.53774134563705722</v>
       </c>
       <c r="H101" s="19">
         <f t="shared" si="11"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="I101" s="19">
         <f t="shared" si="12"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K101" s="2">
         <f t="shared" si="13"/>
@@ -5148,15 +5161,15 @@
       </c>
       <c r="G102" s="19">
         <f t="shared" si="10"/>
-        <v>0.44468877391261652</v>
+        <v>0.50306214938143157</v>
       </c>
       <c r="H102" s="19">
         <f t="shared" si="11"/>
-        <v>0.17526644285268</v>
+        <v>0.2047333884389867</v>
       </c>
       <c r="I102" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K102" s="2">
         <f t="shared" si="13"/>
@@ -5189,11 +5202,11 @@
       </c>
       <c r="G103" s="19">
         <f t="shared" si="10"/>
-        <v>0.39775555271787122</v>
+        <v>0.45274284813652177</v>
       </c>
       <c r="H103" s="19">
         <f t="shared" si="11"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="I103" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5230,11 +5243,11 @@
       </c>
       <c r="G104" s="19">
         <f t="shared" si="10"/>
-        <v>0.35997038776810175</v>
+        <v>0.41168696309760733</v>
       </c>
       <c r="H104" s="19">
         <f t="shared" si="11"/>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="I104" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5271,11 +5284,11 @@
       </c>
       <c r="G105" s="19">
         <f t="shared" si="10"/>
-        <v>0.35997038776810175</v>
+        <v>0.41168696309760733</v>
       </c>
       <c r="H105" s="19">
         <f t="shared" si="11"/>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="I105" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5312,11 +5325,11 @@
       </c>
       <c r="G106" s="19">
         <f t="shared" si="10"/>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="H106" s="19">
         <f t="shared" si="11"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I106" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5353,11 +5366,11 @@
       </c>
       <c r="G107" s="19">
         <f t="shared" si="10"/>
-        <v>0.26977089502064311</v>
+        <v>0.31185700002005889</v>
       </c>
       <c r="H107" s="19">
         <f t="shared" si="11"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="I107" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5394,11 +5407,11 @@
       </c>
       <c r="G108" s="19">
         <f t="shared" si="10"/>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="H108" s="19">
         <f t="shared" si="11"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I108" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5435,11 +5448,11 @@
       </c>
       <c r="G109" s="19">
         <f t="shared" si="10"/>
-        <v>0.28443341673236711</v>
+        <v>0.32825204299627064</v>
       </c>
       <c r="H109" s="19">
         <f t="shared" si="11"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="I109" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5476,11 +5489,11 @@
       </c>
       <c r="G110" s="19">
         <f t="shared" si="10"/>
-        <v>0.26232734853940509</v>
+        <v>0.30351002855087539</v>
       </c>
       <c r="H110" s="19">
         <f t="shared" si="11"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="I110" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5517,11 +5530,11 @@
       </c>
       <c r="G111" s="19">
         <f t="shared" si="10"/>
-        <v>0.3334722374469099</v>
+        <v>0.38261914665522456</v>
       </c>
       <c r="H111" s="19">
         <f t="shared" si="11"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I111" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5558,11 +5571,11 @@
       </c>
       <c r="G112" s="19">
         <f t="shared" si="10"/>
-        <v>0.35997038776810175</v>
+        <v>0.41168696309760733</v>
       </c>
       <c r="H112" s="19">
         <f t="shared" si="11"/>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="I112" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5599,11 +5612,11 @@
       </c>
       <c r="G113" s="19">
         <f t="shared" si="10"/>
-        <v>0.2988015246204283</v>
+        <v>0.34425647321583208</v>
       </c>
       <c r="H113" s="19">
         <f t="shared" si="11"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="I113" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5640,11 +5653,11 @@
       </c>
       <c r="G114" s="19">
         <f t="shared" si="10"/>
-        <v>0.34685567796340067</v>
+        <v>0.39732827778577862</v>
       </c>
       <c r="H114" s="19">
         <f t="shared" si="11"/>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="I114" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5681,11 +5694,11 @@
       </c>
       <c r="G115" s="19">
         <f t="shared" si="10"/>
-        <v>0.31981455971512818</v>
+        <v>0.36755101653626432</v>
       </c>
       <c r="H115" s="19">
         <f t="shared" si="11"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I115" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5722,11 +5735,11 @@
       </c>
       <c r="G116" s="19">
         <f t="shared" si="10"/>
-        <v>0.31981455971512818</v>
+        <v>0.36755101653626432</v>
       </c>
       <c r="H116" s="19">
         <f t="shared" si="11"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I116" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5763,11 +5776,11 @@
       </c>
       <c r="G117" s="19">
         <f t="shared" si="10"/>
-        <v>0.34019789058285854</v>
+        <v>0.39001804768716197</v>
       </c>
       <c r="H117" s="19">
         <f t="shared" si="11"/>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="I117" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5804,15 +5817,15 @@
       </c>
       <c r="G118" s="19">
         <f t="shared" si="10"/>
-        <v>0.31981455971512818</v>
+        <v>0.36755101653626432</v>
       </c>
       <c r="H118" s="19">
         <f t="shared" si="11"/>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="I118" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K118" s="2">
         <f t="shared" si="13"/>
@@ -5845,11 +5858,11 @@
       </c>
       <c r="G119" s="19">
         <f t="shared" si="10"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="H119" s="19">
         <f t="shared" si="11"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="I119" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5886,11 +5899,11 @@
       </c>
       <c r="G120" s="19">
         <f t="shared" si="10"/>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="H120" s="19">
         <f t="shared" si="11"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="I120" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5927,11 +5940,11 @@
       </c>
       <c r="G121" s="19">
         <f t="shared" si="10"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="H121" s="19">
         <f t="shared" si="11"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="I121" s="19" t="str">
         <f t="shared" si="12"/>
@@ -5968,11 +5981,11 @@
       </c>
       <c r="G122" s="19">
         <f t="shared" si="10"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="H122" s="19">
         <f t="shared" si="11"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="I122" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6009,11 +6022,11 @@
       </c>
       <c r="G123" s="19">
         <f t="shared" si="10"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="H123" s="19">
         <f t="shared" si="11"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="I123" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6050,7 +6063,7 @@
       </c>
       <c r="G124" s="19">
         <f t="shared" si="10"/>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="H124" s="19">
         <f t="shared" si="11"/>
@@ -6091,7 +6104,7 @@
       </c>
       <c r="G125" s="19">
         <f t="shared" si="10"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="H125" s="19">
         <f t="shared" si="11"/>
@@ -6132,11 +6145,11 @@
       </c>
       <c r="G126" s="19">
         <f t="shared" si="10"/>
-        <v>0.17526644285268</v>
+        <v>0.2047333884389867</v>
       </c>
       <c r="H126" s="19">
         <f t="shared" si="11"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="I126" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6173,11 +6186,11 @@
       </c>
       <c r="G127" s="19">
         <f t="shared" si="10"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="H127" s="19">
         <f t="shared" si="11"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="I127" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6214,11 +6227,11 @@
       </c>
       <c r="G128" s="19">
         <f t="shared" si="10"/>
-        <v>0.28443341673236711</v>
+        <v>0.32825204299627064</v>
       </c>
       <c r="H128" s="19">
         <f t="shared" si="11"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I128" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6255,11 +6268,11 @@
       </c>
       <c r="G129" s="19">
         <f t="shared" si="10"/>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="H129" s="19">
         <f t="shared" si="11"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="I129" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6296,11 +6309,11 @@
       </c>
       <c r="G130" s="19">
         <f t="shared" si="10"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="H130" s="19">
         <f t="shared" si="11"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="I130" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6337,11 +6350,11 @@
       </c>
       <c r="G131" s="19">
         <f t="shared" si="10"/>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="H131" s="19">
         <f t="shared" si="11"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="I131" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6378,15 +6391,15 @@
       </c>
       <c r="G132" s="19">
         <f t="shared" si="10"/>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="H132" s="19">
         <f t="shared" si="11"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I132" s="19">
         <f t="shared" si="12"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K132" s="2">
         <f t="shared" si="13"/>
@@ -6419,11 +6432,11 @@
       </c>
       <c r="G133" s="19">
         <f t="shared" si="10"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H133" s="19">
         <f t="shared" si="11"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="I133" s="19" t="str">
         <f t="shared" si="12"/>
@@ -6460,11 +6473,11 @@
       </c>
       <c r="G134" s="19">
         <f t="shared" ref="G134:G177" si="19">(1-(1/(2.71828^((C134*($B$1/100))/141))))</f>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="H134" s="19">
         <f t="shared" ref="H134:H177" si="20">(1-(1/(2.71828^((D134*($B$1/100))/141))))</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="I134" s="19" t="str">
         <f t="shared" ref="I134:I177" si="21">IF(E134*($B$1/100)&gt;0, (1-(1/(2.71828^(E134*($B$1/100)/141)))), "&lt;1%")</f>
@@ -6501,15 +6514,15 @@
       </c>
       <c r="G135" s="19">
         <f t="shared" si="19"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="H135" s="19">
         <f t="shared" si="20"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I135" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K135" s="2">
         <f t="shared" si="16"/>
@@ -6542,15 +6555,15 @@
       </c>
       <c r="G136" s="19">
         <f t="shared" si="19"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="H136" s="19">
         <f t="shared" si="20"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I136" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K136" s="2">
         <f t="shared" si="16"/>
@@ -6583,15 +6596,15 @@
       </c>
       <c r="G137" s="19">
         <f t="shared" si="19"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="H137" s="19">
         <f t="shared" si="20"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I137" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K137" s="2">
         <f t="shared" si="16"/>
@@ -6624,15 +6637,15 @@
       </c>
       <c r="G138" s="19">
         <f t="shared" si="19"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="H138" s="19">
         <f t="shared" si="20"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I138" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K138" s="2">
         <f t="shared" si="16"/>
@@ -6665,11 +6678,11 @@
       </c>
       <c r="G139" s="19">
         <f t="shared" si="19"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="H139" s="19">
         <f t="shared" si="20"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="I139" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6706,11 +6719,11 @@
       </c>
       <c r="G140" s="19">
         <f t="shared" si="19"/>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="H140" s="19">
         <f t="shared" si="20"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="I140" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6747,11 +6760,11 @@
       </c>
       <c r="G141" s="19">
         <f t="shared" si="19"/>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="H141" s="19">
         <f t="shared" si="20"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="I141" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6788,11 +6801,11 @@
       </c>
       <c r="G142" s="19">
         <f t="shared" si="19"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="H142" s="19">
         <f t="shared" si="20"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="I142" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6829,11 +6842,11 @@
       </c>
       <c r="G143" s="19">
         <f t="shared" si="19"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="H143" s="19">
         <f t="shared" si="20"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="I143" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6870,11 +6883,11 @@
       </c>
       <c r="G144" s="19">
         <f t="shared" si="19"/>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="H144" s="19">
         <f t="shared" si="20"/>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="I144" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6911,11 +6924,11 @@
       </c>
       <c r="G145" s="19">
         <f t="shared" si="19"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="H145" s="19">
         <f t="shared" si="20"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="I145" s="19" t="str">
         <f t="shared" si="21"/>
@@ -6952,15 +6965,15 @@
       </c>
       <c r="G146" s="19">
         <f t="shared" si="19"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="H146" s="19">
         <f t="shared" si="20"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="I146" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K146" s="2">
         <f t="shared" si="16"/>
@@ -6993,15 +7006,15 @@
       </c>
       <c r="G147" s="19">
         <f t="shared" si="19"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="H147" s="19">
         <f t="shared" si="20"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="I147" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K147" s="2">
         <f t="shared" si="16"/>
@@ -7034,15 +7047,15 @@
       </c>
       <c r="G148" s="19">
         <f t="shared" si="19"/>
-        <v>0.28443341673236711</v>
+        <v>0.32825204299627064</v>
       </c>
       <c r="H148" s="19">
         <f t="shared" si="20"/>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="I148" s="19">
         <f t="shared" si="21"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="K148" s="2">
         <f t="shared" si="16"/>
@@ -7075,15 +7088,15 @@
       </c>
       <c r="G149" s="19">
         <f t="shared" si="19"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H149" s="19">
         <f t="shared" si="20"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I149" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K149" s="2">
         <f t="shared" si="16"/>
@@ -7116,15 +7129,15 @@
       </c>
       <c r="G150" s="19">
         <f t="shared" si="19"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="H150" s="19">
         <f t="shared" si="20"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I150" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K150" s="2">
         <f t="shared" si="16"/>
@@ -7157,11 +7170,11 @@
       </c>
       <c r="G151" s="19">
         <f t="shared" si="19"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H151" s="19">
         <f t="shared" si="20"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I151" s="19" t="str">
         <f t="shared" si="21"/>
@@ -7198,15 +7211,15 @@
       </c>
       <c r="G152" s="19">
         <f t="shared" si="19"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="H152" s="19">
         <f t="shared" si="20"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I152" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K152" s="2">
         <f t="shared" si="16"/>
@@ -7239,15 +7252,15 @@
       </c>
       <c r="G153" s="19">
         <f t="shared" si="19"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="H153" s="19">
         <f t="shared" si="20"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I153" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K153" s="2">
         <f t="shared" si="16"/>
@@ -7280,15 +7293,15 @@
       </c>
       <c r="G154" s="19">
         <f t="shared" si="19"/>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="H154" s="19">
         <f t="shared" si="20"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I154" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K154" s="2">
         <f t="shared" si="16"/>
@@ -7321,15 +7334,15 @@
       </c>
       <c r="G155" s="19">
         <f t="shared" si="19"/>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="H155" s="19">
         <f t="shared" si="20"/>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="I155" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K155" s="2">
         <f t="shared" si="16"/>
@@ -7362,15 +7375,15 @@
       </c>
       <c r="G156" s="19">
         <f t="shared" si="19"/>
-        <v>0.23953835542739466</v>
+        <v>0.27785670909526972</v>
       </c>
       <c r="H156" s="19">
         <f t="shared" si="20"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I156" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K156" s="2">
         <f t="shared" si="16"/>
@@ -7403,15 +7416,15 @@
       </c>
       <c r="G157" s="19">
         <f t="shared" si="19"/>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="H157" s="19">
         <f t="shared" si="20"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I157" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K157" s="2">
         <f t="shared" si="16"/>
@@ -7444,15 +7457,15 @@
       </c>
       <c r="G158" s="19">
         <f t="shared" si="19"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="H158" s="19">
         <f t="shared" si="20"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I158" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K158" s="2">
         <f t="shared" si="16"/>
@@ -7485,15 +7498,15 @@
       </c>
       <c r="G159" s="19">
         <f t="shared" si="19"/>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="H159" s="19">
         <f t="shared" si="20"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="I159" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K159" s="2">
         <f t="shared" si="16"/>
@@ -7526,15 +7539,15 @@
       </c>
       <c r="G160" s="19">
         <f t="shared" si="19"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H160" s="19">
         <f t="shared" si="20"/>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="I160" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K160" s="2">
         <f t="shared" si="16"/>
@@ -7567,15 +7580,15 @@
       </c>
       <c r="G161" s="19">
         <f t="shared" si="19"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="H161" s="19">
         <f t="shared" si="20"/>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="I161" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K161" s="2">
         <f t="shared" si="16"/>
@@ -7608,15 +7621,15 @@
       </c>
       <c r="G162" s="19">
         <f t="shared" si="19"/>
-        <v>0.26977089502064311</v>
+        <v>0.31185700002005889</v>
       </c>
       <c r="H162" s="19">
         <f t="shared" si="20"/>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="I162" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K162" s="2">
         <f t="shared" si="16"/>
@@ -7649,15 +7662,15 @@
       </c>
       <c r="G163" s="19">
         <f t="shared" si="19"/>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H163" s="19">
         <f t="shared" si="20"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I163" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K163" s="2">
         <f t="shared" si="16"/>
@@ -7690,15 +7703,15 @@
       </c>
       <c r="G164" s="19">
         <f t="shared" si="19"/>
-        <v>0.26232734853940509</v>
+        <v>0.30351002855087539</v>
       </c>
       <c r="H164" s="19">
         <f t="shared" si="20"/>
-        <v>0.1323663538771066</v>
+        <v>0.15531728952486967</v>
       </c>
       <c r="I164" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K164" s="2">
         <f t="shared" si="16"/>
@@ -7731,15 +7744,15 @@
       </c>
       <c r="G165" s="19">
         <f t="shared" si="19"/>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="H165" s="19">
         <f t="shared" si="20"/>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="I165" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K165" s="2">
         <f t="shared" si="16"/>
@@ -7772,15 +7785,15 @@
       </c>
       <c r="G166" s="19">
         <f t="shared" si="19"/>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="H166" s="19">
         <f t="shared" si="20"/>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="I166" s="19">
         <f t="shared" si="21"/>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="K166" s="2">
         <f t="shared" si="16"/>
@@ -7813,15 +7826,15 @@
       </c>
       <c r="G167" s="19">
         <f t="shared" si="19"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="H167" s="19">
         <f t="shared" si="20"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I167" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K167" s="2">
         <f t="shared" si="16"/>
@@ -7854,15 +7867,15 @@
       </c>
       <c r="G168" s="19">
         <f t="shared" si="19"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="H168" s="19">
         <f t="shared" si="20"/>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="I168" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K168" s="2">
         <f t="shared" si="16"/>
@@ -7895,15 +7908,15 @@
       </c>
       <c r="G169" s="19">
         <f t="shared" si="19"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="H169" s="19">
         <f t="shared" si="20"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="I169" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K169" s="2">
         <f t="shared" si="16"/>
@@ -7936,15 +7949,15 @@
       </c>
       <c r="G170" s="19">
         <f t="shared" si="19"/>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="H170" s="19">
         <f t="shared" si="20"/>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="I170" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K170" s="2">
         <f t="shared" si="16"/>
@@ -7977,11 +7990,11 @@
       </c>
       <c r="G171" s="19">
         <f t="shared" si="19"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="H171" s="19">
         <f t="shared" si="20"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="I171" s="19" t="str">
         <f t="shared" si="21"/>
@@ -8018,11 +8031,11 @@
       </c>
       <c r="G172" s="19">
         <f t="shared" si="19"/>
-        <v>0.15836700404317228</v>
+        <v>0.18532368255428877</v>
       </c>
       <c r="H172" s="19">
         <f t="shared" si="20"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="I172" s="19" t="str">
         <f t="shared" si="21"/>
@@ -8059,11 +8072,11 @@
       </c>
       <c r="G173" s="19">
         <f t="shared" si="19"/>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="H173" s="19">
         <f t="shared" si="20"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="I173" s="19" t="str">
         <f t="shared" si="21"/>
@@ -8100,15 +8113,15 @@
       </c>
       <c r="G174" s="19">
         <f t="shared" si="19"/>
-        <v>0.18358848455384336</v>
+        <v>0.21426413258348997</v>
       </c>
       <c r="H174" s="19">
         <f t="shared" si="20"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="I174" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K174" s="2">
         <f t="shared" si="16"/>
@@ -8141,15 +8154,15 @@
       </c>
       <c r="G175" s="19">
         <f t="shared" si="19"/>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="H175" s="19">
         <f t="shared" si="20"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="I175" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K175" s="2">
         <f t="shared" si="16"/>
@@ -8182,15 +8195,15 @@
       </c>
       <c r="G176" s="19">
         <f t="shared" si="19"/>
-        <v>0.16685957091974546</v>
+        <v>0.19508703918121972</v>
       </c>
       <c r="H176" s="19">
         <f t="shared" si="20"/>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="I176" s="19">
         <f t="shared" si="21"/>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="K176" s="2">
         <f t="shared" si="16"/>
@@ -8223,11 +8236,11 @@
       </c>
       <c r="G177" s="19">
         <f t="shared" si="19"/>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="H177" s="19">
         <f t="shared" si="20"/>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="I177" s="19" t="str">
         <f t="shared" si="21"/>
@@ -10917,30 +10930,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.625" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="31.25" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13" max="22" width="7.6640625" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="12.6640625" style="1"/>
+    <col min="10" max="10" width="15.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" style="1" customWidth="1"/>
+    <col min="13" max="22" width="7.625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="12.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="19"/>
-      <c r="G1" s="22">
-        <v>2021</v>
+      <c r="G1" s="22" t="s">
+        <v>232</v>
       </c>
       <c r="H1" s="19"/>
       <c r="J1" s="10"/>
@@ -10949,7 +10964,7 @@
       </c>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>228</v>
       </c>
@@ -10978,7 +10993,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -11010,7 +11025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -11025,15 +11040,15 @@
       </c>
       <c r="F4" s="2">
         <f>(1-(1/(2.71828^((B4*(County!$B$1/100))/141))))</f>
-        <v>0.74046516355819192</v>
+        <v>0.79881794219674895</v>
       </c>
       <c r="G4" s="2">
         <f>(1-(1/(2.71828^((C4*(County!$B$1/100))/141))))</f>
-        <v>0.47747245434733998</v>
+        <v>0.53774134563705722</v>
       </c>
       <c r="H4" s="2">
         <f>IF(D4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="J4" s="2">
         <f>(1-(1/(2.71828^(B4/141))))</f>
@@ -11048,7 +11063,7 @@
         <v>0.15651457088727549</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -11063,15 +11078,15 @@
       </c>
       <c r="F5" s="2">
         <f>(1-(1/(2.71828^((B5*(County!$B$1/100))/141))))</f>
-        <v>0.78377103500559842</v>
+        <v>0.83806595418997021</v>
       </c>
       <c r="G5" s="2">
         <f>(1-(1/(2.71828^((C5*(County!$B$1/100))/141))))</f>
-        <v>0.4982458027801665</v>
+        <v>0.55950562556431493</v>
       </c>
       <c r="H5" s="2">
         <f>IF(D5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ref="J5:J21" si="0">(1-(1/(2.71828^(B5/141))))</f>
@@ -11086,7 +11101,7 @@
         <v>0.14446499067653729</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -11101,15 +11116,15 @@
       </c>
       <c r="F6" s="2">
         <f>(1-(1/(2.71828^((B6*(County!$B$1/100))/141))))</f>
-        <v>0.65871410044924505</v>
+        <v>0.72140978066665684</v>
       </c>
       <c r="G6" s="2">
         <f>(1-(1/(2.71828^((C6*(County!$B$1/100))/141))))</f>
-        <v>0.37915035631580263</v>
+        <v>0.43258611492195864</v>
       </c>
       <c r="H6" s="2">
         <f>IF(D6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
@@ -11124,7 +11139,7 @@
         <v>7.5048644888033755E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -11139,15 +11154,15 @@
       </c>
       <c r="F7" s="2">
         <f>(1-(1/(2.71828^((B7*(County!$B$1/100))/141))))</f>
-        <v>0.71276252588327726</v>
+        <v>0.77303914603711887</v>
       </c>
       <c r="G7" s="2">
         <f>(1-(1/(2.71828^((C7*(County!$B$1/100))/141))))</f>
-        <v>0.37282176279753421</v>
+        <v>0.425703551980676</v>
       </c>
       <c r="H7" s="2">
         <f>IF(D7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
@@ -11162,7 +11177,7 @@
         <v>8.158537189746129E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -11177,15 +11192,15 @@
       </c>
       <c r="F8" s="2">
         <f>(1-(1/(2.71828^((B8*(County!$B$1/100))/141))))</f>
-        <v>0.93789093826413483</v>
+        <v>0.9632473106772913</v>
       </c>
       <c r="G8" s="2">
         <f>(1-(1/(2.71828^((C8*(County!$B$1/100))/141))))</f>
-        <v>0.6884860854390159</v>
+        <v>0.75005737564642649</v>
       </c>
       <c r="H8" s="2">
         <f>IF(D8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.38541509064135093</v>
+        <v>0.43938619490029751</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
@@ -11200,7 +11215,7 @@
         <v>0.2885323308745229</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>69</v>
       </c>
@@ -11215,15 +11230,15 @@
       </c>
       <c r="F9" s="2">
         <f>(1-(1/(2.71828^((B9*(County!$B$1/100))/141))))</f>
-        <v>0.75825146410807087</v>
+        <v>0.81510036728918622</v>
       </c>
       <c r="G9" s="2">
         <f>(1-(1/(2.71828^((C9*(County!$B$1/100))/141))))</f>
-        <v>0.40383254978091254</v>
+        <v>0.45930136300416158</v>
       </c>
       <c r="H9" s="2">
         <f>IF(D9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
@@ -11238,7 +11253,7 @@
         <v>6.1835286174562576E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>76</v>
       </c>
@@ -11253,15 +11268,15 @@
       </c>
       <c r="F10" s="2">
         <f>(1-(1/(2.71828^((B10*(County!$B$1/100))/141))))</f>
-        <v>0.69782132082385306</v>
+        <v>0.7589363032344425</v>
       </c>
       <c r="G10" s="2">
         <f>(1-(1/(2.71828^((C10*(County!$B$1/100))/141))))</f>
-        <v>0.38541509064135093</v>
+        <v>0.43938619490029751</v>
       </c>
       <c r="H10" s="2">
         <f>IF(D10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
@@ -11276,7 +11291,7 @@
         <v>8.158537189746129E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>83</v>
       </c>
@@ -11291,15 +11306,15 @@
       </c>
       <c r="F11" s="2">
         <f>(1-(1/(2.71828^((B11*(County!$B$1/100))/141))))</f>
-        <v>0.80062187005869268</v>
+        <v>0.85295549561519524</v>
       </c>
       <c r="G11" s="2">
         <f>(1-(1/(2.71828^((C11*(County!$B$1/100))/141))))</f>
-        <v>0.4982458027801665</v>
+        <v>0.55950562556431493</v>
       </c>
       <c r="H11" s="2">
         <f>IF(D11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D11*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
@@ -11314,7 +11329,7 @@
         <v>7.5048644888033755E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>92</v>
       </c>
@@ -11329,15 +11344,15 @@
       </c>
       <c r="F12" s="2">
         <f>(1-(1/(2.71828^((B12*(County!$B$1/100))/141))))</f>
-        <v>0.58196829283544926</v>
+        <v>0.64544036884895628</v>
       </c>
       <c r="G12" s="2">
         <f>(1-(1/(2.71828^((C12*(County!$B$1/100))/141))))</f>
-        <v>0.26977089502064311</v>
+        <v>0.31185700002005889</v>
       </c>
       <c r="H12" s="2">
         <f>IF(D12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D12*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
@@ -11352,7 +11367,7 @@
         <v>1.408426315629896E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>95</v>
       </c>
@@ -11367,15 +11382,15 @@
       </c>
       <c r="F13" s="2">
         <f>(1-(1/(2.71828^((B13*(County!$B$1/100))/141))))</f>
-        <v>0.4098482264059311</v>
+        <v>0.46578127841061079</v>
       </c>
       <c r="G13" s="2">
         <f>(1-(1/(2.71828^((C13*(County!$B$1/100))/141))))</f>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="H13" s="2">
         <f>IF(D13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
@@ -11390,7 +11405,7 @@
         <v>7.0671035544741523E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>97</v>
       </c>
@@ -11405,15 +11420,15 @@
       </c>
       <c r="F14" s="2">
         <f>(1-(1/(2.71828^((B14*(County!$B$1/100))/141))))</f>
-        <v>0.30587702543196937</v>
+        <v>0.3521151255059447</v>
       </c>
       <c r="G14" s="2">
         <f>(1-(1/(2.71828^((C14*(County!$B$1/100))/141))))</f>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="H14" s="2">
         <f>IF(D14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
@@ -11428,7 +11443,7 @@
         <v>7.0671035544741523E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>99</v>
       </c>
@@ -11443,15 +11458,15 @@
       </c>
       <c r="F15" s="2">
         <f>(1-(1/(2.71828^((B15*(County!$B$1/100))/141))))</f>
-        <v>0.30587702543196937</v>
+        <v>0.3521151255059447</v>
       </c>
       <c r="G15" s="2">
         <f>(1-(1/(2.71828^((C15*(County!$B$1/100))/141))))</f>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="H15" s="2">
         <f>IF(D15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
@@ -11466,7 +11481,7 @@
         <v>7.0671035544741523E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>104</v>
       </c>
@@ -11481,15 +11496,15 @@
       </c>
       <c r="F16" s="2">
         <f>(1-(1/(2.71828^((B16*(County!$B$1/100))/141))))</f>
-        <v>0.35344628439351555</v>
+        <v>0.40455089961354063</v>
       </c>
       <c r="G16" s="2">
         <f>(1-(1/(2.71828^((C16*(County!$B$1/100))/141))))</f>
-        <v>0.1323663538771066</v>
+        <v>0.15531728952486967</v>
       </c>
       <c r="H16" s="2">
         <f>IF(D16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D16*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
@@ -11504,7 +11519,7 @@
         <v>2.1051831764559048E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>129</v>
       </c>
@@ -11519,15 +11534,15 @@
       </c>
       <c r="F17" s="2">
         <f>(1-(1/(2.71828^((B17*(County!$B$1/100))/141))))</f>
-        <v>0.2988015246204283</v>
+        <v>0.34425647321583208</v>
       </c>
       <c r="G17" s="2">
         <f>(1-(1/(2.71828^((C17*(County!$B$1/100))/141))))</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="H17" s="2">
         <f>IF(D17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
@@ -11542,7 +11557,7 @@
         <v>1.408426315629896E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>108</v>
       </c>
@@ -11557,15 +11572,15 @@
       </c>
       <c r="F18" s="2">
         <f>(1-(1/(2.71828^((B18*(County!$B$1/100))/141))))</f>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="G18" s="2">
         <f>(1-(1/(2.71828^((C18*(County!$B$1/100))/141))))</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="H18" s="2">
         <f>IF(D18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
@@ -11580,7 +11595,7 @@
         <v>1.408426315629896E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>112</v>
       </c>
@@ -11595,15 +11610,15 @@
       </c>
       <c r="F19" s="2">
         <f>(1-(1/(2.71828^((B19*(County!$B$1/100))/141))))</f>
-        <v>0.43331001042692008</v>
+        <v>0.49093361615337672</v>
       </c>
       <c r="G19" s="2">
         <f>(1-(1/(2.71828^((C19*(County!$B$1/100))/141))))</f>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="H19" s="2">
         <f>IF(D19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
@@ -11633,15 +11648,15 @@
       </c>
       <c r="F20" s="2">
         <f>(1-(1/(2.71828^((B20*(County!$B$1/100))/141))))</f>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="G20" s="2">
         <f>(1-(1/(2.71828^((C20*(County!$B$1/100))/141))))</f>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="H20" s="2">
         <f>IF(D20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="0"/>
@@ -11671,15 +11686,15 @@
       </c>
       <c r="F21" s="2">
         <f>(1-(1/(2.71828^((B21*(County!$B$1/100))/141))))</f>
-        <v>0.2916539001167342</v>
+        <v>0.33630249779309462</v>
       </c>
       <c r="G21" s="2">
         <f>(1-(1/(2.71828^((C21*(County!$B$1/100))/141))))</f>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="H21" s="2">
         <f>IF(D21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
@@ -12683,29 +12698,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DAC7B-140A-4EB4-AEF9-29CE074480FA}">
   <dimension ref="A1:L982"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.25" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.75" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="7.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="12.6640625" style="1"/>
+    <col min="13" max="15" width="7.625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="12.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="19"/>
       <c r="G1" s="22">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="H1" s="19"/>
       <c r="J1" s="10"/>
@@ -12714,7 +12731,7 @@
       </c>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>228</v>
       </c>
@@ -12743,7 +12760,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>130</v>
       </c>
@@ -12775,7 +12792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>131</v>
       </c>
@@ -12790,15 +12807,15 @@
       </c>
       <c r="F4" s="3">
         <f>IF(B4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.43902824231404158</v>
+        <v>0.49703443993558749</v>
       </c>
       <c r="G4" s="3">
         <f>IF(C4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="H4" s="3">
         <f>IF(D4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J4" s="3">
         <f>(1-(1/(2.71828^(B4/141))))</f>
@@ -12813,7 +12830,7 @@
         <v>7.0671035544741523E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>132</v>
       </c>
@@ -12828,15 +12845,15 @@
       </c>
       <c r="F5" s="3">
         <f>IF(B5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.54201619718511251</v>
+        <v>0.6048019193821581</v>
       </c>
       <c r="G5" s="3">
         <f>IF(C5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.35997038776810175</v>
+        <v>0.41168696309760733</v>
       </c>
       <c r="H5" s="3">
         <f>IF(D5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:K7" si="0">(1-(1/(2.71828^(B5/141))))</f>
@@ -12851,7 +12868,7 @@
         <v>7.0671035544741523E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>133</v>
       </c>
@@ -12866,11 +12883,11 @@
       </c>
       <c r="F6" s="3">
         <f>IF(B6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.1323663538771066</v>
+        <v>0.15531728952486967</v>
       </c>
       <c r="G6" s="3">
         <f>IF(C6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="H6" s="3" t="str">
         <f>IF(D6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D6*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -12889,7 +12906,7 @@
         <v>&lt;1%</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>134</v>
       </c>
@@ -12904,15 +12921,15 @@
       </c>
       <c r="F7" s="3">
         <f>IF(B7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.35344628439351555</v>
+        <v>0.40455089961354063</v>
       </c>
       <c r="G7" s="3">
         <f>IF(C7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.21604533973025641</v>
+        <v>0.2512585191805502</v>
       </c>
       <c r="H7" s="3">
         <f>IF(D7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
@@ -13912,29 +13929,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9E57B6-B9DF-451B-AC8D-7B7640F6A107}">
   <dimension ref="A1:L1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.25" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.75" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="7.6640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="12.6640625" style="1"/>
+    <col min="13" max="18" width="7.625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="12.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F1" s="19"/>
       <c r="G1" s="22">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="H1" s="19"/>
       <c r="J1" s="10"/>
@@ -13943,7 +13962,7 @@
       </c>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>228</v>
       </c>
@@ -14019,15 +14038,15 @@
       </c>
       <c r="F4" s="3">
         <f>IF(B4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.46132995995618065</v>
+        <v>0.52071530159105595</v>
       </c>
       <c r="G4" s="3">
         <f>IF(C4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="H4" s="3">
         <f>IF(D4*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D4*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="J4" s="3">
         <f>(1-(1/(2.71828^(B4/141))))</f>
@@ -14057,15 +14076,15 @@
       </c>
       <c r="F5" s="3">
         <f>IF(B5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.37282176279753421</v>
+        <v>0.425703551980676</v>
       </c>
       <c r="G5" s="3">
         <f>IF(C5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H5" s="3">
         <f>IF(D5*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D5*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:K7" si="0">(1-(1/(2.71828^(B5/141))))</f>
@@ -14095,11 +14114,11 @@
       </c>
       <c r="F6" s="3">
         <f>IF(B6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="G6" s="3">
         <f>IF(C6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C6*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>6.8531457255322281E-2</v>
+        <v>8.0933783411047955E-2</v>
       </c>
       <c r="H6" s="3" t="str">
         <f>IF(D6*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D6*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14133,15 +14152,15 @@
       </c>
       <c r="F7" s="3">
         <f>IF(B7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.90960943662496641</v>
+        <v>0.94258472444679964</v>
       </c>
       <c r="G7" s="3">
         <f>IF(C7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.65871410044924505</v>
+        <v>0.72140978066665684</v>
       </c>
       <c r="H7" s="3">
         <f>IF(D7*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D7*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.39775555271787122</v>
+        <v>0.45274284813652177</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
@@ -14171,15 +14190,15 @@
       </c>
       <c r="F8" s="3">
         <f>IF(B8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.37915035631580263</v>
+        <v>0.43258611492195864</v>
       </c>
       <c r="G8" s="3">
         <f>IF(C8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="H8" s="3">
         <f>IF(D8*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D8*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ref="J8:J41" si="2">(1-(1/(2.71828^(B8/141))))</f>
@@ -14209,15 +14228,15 @@
       </c>
       <c r="F9" s="3">
         <f>IF(B9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.53734776682447505</v>
+        <v>0.60000828331568745</v>
       </c>
       <c r="G9" s="3">
         <f>IF(C9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.26232734853940509</v>
+        <v>0.30351002855087539</v>
       </c>
       <c r="H9" s="3">
         <f>IF(D9*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D9*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="2"/>
@@ -14247,15 +14266,15 @@
       </c>
       <c r="F10" s="3">
         <f>IF(B10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.51328202850696369</v>
+        <v>0.57515368744915019</v>
       </c>
       <c r="G10" s="3">
         <f>IF(C10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.34685567796340067</v>
+        <v>0.39732827778577862</v>
       </c>
       <c r="H10" s="3">
         <f>IF(D10*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D10*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.15836700404317228</v>
+        <v>0.18532368255428877</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="2"/>
@@ -14285,11 +14304,11 @@
       </c>
       <c r="F11" s="3">
         <f>IF(B11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B11*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="G11" s="3">
         <f>IF(C11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C11*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="H11" s="3" t="str">
         <f>IF(D11*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D11*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14323,11 +14342,11 @@
       </c>
       <c r="F12" s="3">
         <f>IF(B12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B12*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="G12" s="3">
         <f>IF(C12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C12*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="H12" s="3" t="str">
         <f>IF(D12*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D12*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14361,15 +14380,15 @@
       </c>
       <c r="F13" s="3">
         <f>IF(B13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.51328202850696369</v>
+        <v>0.57515368744915019</v>
       </c>
       <c r="G13" s="3">
         <f>IF(C13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.31288113032139719</v>
+        <v>0.3598795970481059</v>
       </c>
       <c r="H13" s="3">
         <f>IF(D13*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D13*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="2"/>
@@ -14399,15 +14418,15 @@
       </c>
       <c r="F14" s="3">
         <f>IF(B14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="G14" s="3">
         <f>IF(C14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="H14" s="3">
         <f>IF(D14*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D14*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="2"/>
@@ -14437,15 +14456,15 @@
       </c>
       <c r="F15" s="3">
         <f>IF(B15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.87367973087526618</v>
+        <v>0.91452854459089683</v>
       </c>
       <c r="G15" s="3">
         <f>IF(C15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.64458437129927193</v>
+        <v>0.70764498395084252</v>
       </c>
       <c r="H15" s="3">
         <f>IF(D15*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D15*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.34019789058285854</v>
+        <v>0.39001804768716197</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="2"/>
@@ -14475,11 +14494,11 @@
       </c>
       <c r="F16" s="3">
         <f>IF(B16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B16*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="G16" s="3">
         <f>IF(C16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C16*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="H16" s="3" t="str">
         <f>IF(D16*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D16*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -14513,15 +14532,15 @@
       </c>
       <c r="F17" s="3">
         <f>IF(B17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.43902824231404158</v>
+        <v>0.49703443993558749</v>
       </c>
       <c r="G17" s="3">
         <f>IF(C17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.19182655200965715</v>
+        <v>0.22368065706552087</v>
       </c>
       <c r="H17" s="3">
         <f>IF(D17*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D17*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="2"/>
@@ -14551,15 +14570,15 @@
       </c>
       <c r="F18" s="3">
         <f>IF(B18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.71276252588327726</v>
+        <v>0.77303914603711887</v>
       </c>
       <c r="G18" s="3">
         <f>IF(C18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.46132995995618065</v>
+        <v>0.52071530159105595</v>
       </c>
       <c r="H18" s="3">
         <f>IF(D18*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D18*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.23178663537135147</v>
+        <v>0.26909732413310372</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="2"/>
@@ -14589,15 +14608,15 @@
       </c>
       <c r="F19" s="3">
         <f>IF(B19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.37282176279753421</v>
+        <v>0.425703551980676</v>
       </c>
       <c r="G19" s="3">
         <f>IF(C19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="H19" s="3">
         <f>IF(D19*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D19*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" si="2"/>
@@ -14627,15 +14646,15 @@
       </c>
       <c r="F20" s="3">
         <f>IF(B20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="G20" s="3">
         <f>IF(C20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.2472118561154939</v>
+        <v>0.28651111862438716</v>
       </c>
       <c r="H20" s="3">
         <f>IF(D20*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D20*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>9.6445067831425813E-2</v>
+        <v>0.11358256593379767</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" si="2"/>
@@ -14665,15 +14684,15 @@
       </c>
       <c r="F21" s="3">
         <f>IF(B21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.4982458027801665</v>
+        <v>0.55950562556431493</v>
       </c>
       <c r="G21" s="3">
         <f>IF(C21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H21" s="3">
         <f>IF(D21*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D21*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>3.9755508787349569E-2</v>
+        <v>4.7082471516410873E-2</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" si="2"/>
@@ -14703,15 +14722,15 @@
       </c>
       <c r="F22" s="3">
         <f>IF(B22*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B22*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.56466117640869062</v>
+        <v>0.62792201785261859</v>
       </c>
       <c r="G22" s="3">
         <f>IF(C22*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C22*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.34685567796340067</v>
+        <v>0.39732827778577862</v>
       </c>
       <c r="H22" s="3">
         <f>IF(D22*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D22*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.1323663538771066</v>
+        <v>0.15531728952486967</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" si="2"/>
@@ -14741,15 +14760,15 @@
       </c>
       <c r="F23" s="3">
         <f>IF(B23*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B23*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.77252347298151669</v>
+        <v>0.82800373265447247</v>
       </c>
       <c r="G23" s="3">
         <f>IF(C23*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C23*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.37282176279753421</v>
+        <v>0.425703551980676</v>
       </c>
       <c r="H23" s="3">
         <f>IF(D23*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D23*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" si="2"/>
@@ -14779,15 +14798,15 @@
       </c>
       <c r="F24" s="3">
         <f>IF(B24*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B24*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.59036209546628593</v>
+        <v>0.65388777061068404</v>
       </c>
       <c r="G24" s="3">
         <f>IF(C24*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C24*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.30587702543196937</v>
+        <v>0.3521151255059447</v>
       </c>
       <c r="H24" s="3">
         <f>IF(D24*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D24*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="2"/>
@@ -14817,15 +14836,15 @@
       </c>
       <c r="F25" s="3">
         <f>IF(B25*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B25*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="G25" s="3">
         <f>IF(C25*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C25*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.15836700404317228</v>
+        <v>0.18532368255428877</v>
       </c>
       <c r="H25" s="3">
         <f>IF(D25*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D25*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>5.9036588663461731E-2</v>
+        <v>6.9785781486474296E-2</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" si="2"/>
@@ -14855,15 +14874,15 @@
       </c>
       <c r="F26" s="3">
         <f>IF(B26*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B26*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.87367973087526618</v>
+        <v>0.91452854459089683</v>
       </c>
       <c r="G26" s="3">
         <f>IF(C26*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C26*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.56905399856642302</v>
+        <v>0.63238112628002896</v>
       </c>
       <c r="H26" s="3">
         <f>IF(D26*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D26*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.25480792671460639</v>
+        <v>0.29506181078156346</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" si="2"/>
@@ -14893,15 +14912,15 @@
       </c>
       <c r="F27" s="3">
         <f>IF(B27*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B27*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.35344628439351555</v>
+        <v>0.40455089961354063</v>
       </c>
       <c r="G27" s="3">
         <f>IF(C27*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C27*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.19998149256914177</v>
+        <v>0.23298433073215996</v>
       </c>
       <c r="H27" s="3">
         <f>IF(D27*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D27*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>7.7930517095758045E-2</v>
+        <v>9.1948183908728165E-2</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="2"/>
@@ -14931,15 +14950,15 @@
       </c>
       <c r="F28" s="3">
         <f>IF(B28*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B28*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.46676545424104743</v>
+        <v>0.52645921157860687</v>
       </c>
       <c r="G28" s="3">
         <f>IF(C28*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C28*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.22395589862293985</v>
+        <v>0.26023169041687233</v>
       </c>
       <c r="H28" s="3">
         <f>IF(D28*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D28*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="2"/>
@@ -14969,11 +14988,11 @@
       </c>
       <c r="F29" s="3">
         <f>IF(B29*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B29*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="G29" s="3">
         <f>IF(C29*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C29*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>1.009058213897418E-2</v>
+        <v>1.1984338341321177E-2</v>
       </c>
       <c r="H29" s="3" t="str">
         <f>IF(D29*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D29*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -15007,15 +15026,15 @@
       </c>
       <c r="F30" s="3">
         <f>IF(B30*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B30*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.52305500629686519</v>
+        <v>0.585275673072428</v>
       </c>
       <c r="G30" s="3">
         <f>IF(C30*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C30*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.31981455971512818</v>
+        <v>0.36755101653626432</v>
       </c>
       <c r="H30" s="3">
         <f>IF(D30*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D30*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.1323663538771066</v>
+        <v>0.15531728952486967</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" si="2"/>
@@ -15045,15 +15064,15 @@
       </c>
       <c r="F31" s="3">
         <f>IF(B31*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B31*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.32667802677005708</v>
+        <v>0.37513049913771845</v>
       </c>
       <c r="G31" s="3">
         <f>IF(C31*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C31*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H31" s="3">
         <f>IF(D31*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D31*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>8.7234734950844883E-2</v>
+        <v>0.10283058410421708</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="2"/>
@@ -15083,15 +15102,15 @@
       </c>
       <c r="F32" s="3">
         <f>IF(B32*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B32*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.45029218745214572</v>
+        <v>0.5090176207178535</v>
       </c>
       <c r="G32" s="3">
         <f>IF(C32*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C32*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="H32" s="3">
         <f>IF(D32*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D32*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" si="2"/>
@@ -15121,15 +15140,15 @@
       </c>
       <c r="F33" s="3">
         <f>IF(B33*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B33*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.52305500629686519</v>
+        <v>0.585275673072428</v>
       </c>
       <c r="G33" s="3">
         <f>IF(C33*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C33*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="H33" s="3">
         <f>IF(D33*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D33*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>4.9444934699428233E-2</v>
+        <v>5.8502557589133808E-2</v>
       </c>
       <c r="J33" s="3">
         <f t="shared" si="2"/>
@@ -15159,15 +15178,15 @@
       </c>
       <c r="F34" s="3">
         <f>IF(B34*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B34*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.35344628439351555</v>
+        <v>0.40455089961354063</v>
       </c>
       <c r="G34" s="3">
         <f>IF(C34*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C34*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H34" s="3">
         <f>IF(D34*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D34*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="J34" s="3">
         <f t="shared" si="2"/>
@@ -15197,15 +15216,15 @@
       </c>
       <c r="F35" s="3">
         <f>IF(B35*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B35*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.52786765893159926</v>
+        <v>0.59024586972470483</v>
       </c>
       <c r="G35" s="3">
         <f>IF(C35*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C35*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.12352218246629398</v>
+        <v>0.1450715375735252</v>
       </c>
       <c r="H35" s="3">
         <f>IF(D35*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D35*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.0079344430044999E-2</v>
+        <v>2.3825052317163253E-2</v>
       </c>
       <c r="J35" s="3">
         <f t="shared" si="2"/>
@@ -15235,15 +15254,15 @@
       </c>
       <c r="F36" s="3">
         <f>IF(B36*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B36*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.3334722374469099</v>
+        <v>0.38261914665522456</v>
       </c>
       <c r="G36" s="3">
         <f>IF(C36*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C36*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H36" s="3">
         <f>IF(D36*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D36*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" si="2"/>
@@ -15273,15 +15292,15 @@
       </c>
       <c r="F37" s="3">
         <f>IF(B37*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B37*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.35344628439351555</v>
+        <v>0.40455089961354063</v>
       </c>
       <c r="G37" s="3">
         <f>IF(C37*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C37*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.20805414503107234</v>
+        <v>0.24217650602576057</v>
       </c>
       <c r="H37" s="3">
         <f>IF(D37*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D37*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="J37" s="3">
         <f t="shared" si="2"/>
@@ -15311,11 +15330,11 @@
       </c>
       <c r="F38" s="3">
         <f>IF(B38*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B38*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.10556246309154804</v>
+        <v>0.12420569237529278</v>
       </c>
       <c r="G38" s="3">
         <f>IF(C38*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C38*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>2.996731429475108E-2</v>
+        <v>3.5523863170515813E-2</v>
       </c>
       <c r="H38" s="3" t="str">
         <f>IF(D38*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D38*(County!$B$1/100)/141)))), "&lt;1%")</f>
@@ -15349,15 +15368,15 @@
       </c>
       <c r="F39" s="3">
         <f>IF(B39*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B39*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.52305500629686519</v>
+        <v>0.585275673072428</v>
       </c>
       <c r="G39" s="3">
         <f>IF(C39*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C39*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.27713933178470684</v>
+        <v>0.32010393855903041</v>
       </c>
       <c r="H39" s="3">
         <f>IF(D39*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D39*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.14978786869670402</v>
+        <v>0.17544189929334297</v>
       </c>
       <c r="J39" s="3">
         <f t="shared" si="2"/>
@@ -15387,15 +15406,15 @@
       </c>
       <c r="F40" s="3">
         <f>IF(B40*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B40*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.50330879472078838</v>
+        <v>0.56478465918500087</v>
       </c>
       <c r="G40" s="3">
         <f>IF(C40*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C40*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.2988015246204283</v>
+        <v>0.34425647321583208</v>
       </c>
       <c r="H40" s="3">
         <f>IF(D40*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D40*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.14112128244984734</v>
+        <v>0.16544025291826803</v>
       </c>
       <c r="J40" s="3">
         <f t="shared" si="2"/>
@@ -15425,15 +15444,15 @@
       </c>
       <c r="F41" s="3">
         <f>IF(B41*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(B41*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.43902824231404158</v>
+        <v>0.49703443993558749</v>
       </c>
       <c r="G41" s="3">
         <f>IF(C41*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(C41*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.26232734853940509</v>
+        <v>0.30351002855087539</v>
       </c>
       <c r="H41" s="3">
         <f>IF(D41*(County!$B$1/100)&gt;0, (1-(1/(2.71828^(D41*(County!$B$1/100)/141)))), "&lt;1%")</f>
-        <v>0.11458785852590458</v>
+        <v>0.13470150767527056</v>
       </c>
       <c r="J41" s="3">
         <f t="shared" si="2"/>

</xml_diff>